<commit_message>
uploaded inventory usecase diagram and flowchart
these are first drafts just hand drawn out
</commit_message>
<xml_diff>
--- a/docs/Database Tables Outlines/POS - Database Tracker.xlsx
+++ b/docs/Database Tables Outlines/POS - Database Tracker.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10911"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\CPS353-POS\docs\Database Tables Outlines\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/XAMPP/xamppfiles/htdocs/CPS353-POS/docs/Database Tables Outlines/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84218E5D-7A0F-4081-8C52-E7303ABC5595}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C41DFE68-2EED-7E47-A83F-A55B94F2F527}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DOCS" sheetId="3" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1347" uniqueCount="467">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1390" uniqueCount="468">
   <si>
     <t xml:space="preserve">table name </t>
   </si>
@@ -1701,6 +1701,9 @@
   </si>
   <si>
     <t>not_registered</t>
+  </si>
+  <si>
+    <t>ç</t>
   </si>
 </sst>
 </file>
@@ -2255,6 +2258,37 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -2305,37 +2339,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3593,6 +3596,40 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="25" xr:uid="{DFF8B94E-191D-9C40-BBAF-0B8A40F97BF0}" name="Table15526" displayName="Table15526" ref="D9:E14" totalsRowShown="0">
+  <autoFilter ref="D9:E14" xr:uid="{DFF8B94E-191D-9C40-BBAF-0B8A40F97BF0}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{4D2D2720-BA12-4B4C-A04F-B3D2DB0B2F3D}" name="sales_details"/>
+    <tableColumn id="2" xr3:uid="{6967D3E5-8319-DA42-BF2B-F54307F6206C}" name="Column1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="26" xr:uid="{1F308ECC-2FA6-2148-A0F9-C72181D4B135}" name="Table91527" displayName="Table91527" ref="G9:I15" totalsRowShown="0">
+  <autoFilter ref="G9:I15" xr:uid="{1F308ECC-2FA6-2148-A0F9-C72181D4B135}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{8D42ECBB-047F-0C4A-986A-D29CDD20DCDF}" name="prod_sales"/>
+    <tableColumn id="2" xr3:uid="{41E7D70D-B061-2D4C-ADBD-E7010CB23182}" name="Column1"/>
+    <tableColumn id="3" xr3:uid="{32D12888-6453-7543-9448-D625A827EC8B}" name="ç"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{EEE9A7FF-A6ED-4209-A1C4-CC197F0AC95C}" name="Table11" displayName="Table11" ref="A7:B15" totalsRowShown="0">
+  <autoFilter ref="A7:B15" xr:uid="{EEE9A7FF-A6ED-4209-A1C4-CC197F0AC95C}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{A70E2D6B-6988-49C6-B102-5D940C03D8A4}" name="invoice"/>
+    <tableColumn id="2" xr3:uid="{4D9C4735-0D32-45DB-B042-737ABFC2EBD5}" name="datatype"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{15B03442-C8BD-9645-8390-80E2FF8FDE57}" name="Table155" displayName="Table155" ref="D7:E12" totalsRowShown="0">
   <autoFilter ref="D7:E12" xr:uid="{15B03442-C8BD-9645-8390-80E2FF8FDE57}"/>
   <tableColumns count="2">
@@ -3603,18 +3640,19 @@
 </table>
 </file>
 
-<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{C2E51D9C-415E-A840-96CF-42A4AD54C811}" name="Table915" displayName="Table915" ref="G7:H13" totalsRowShown="0">
-  <autoFilter ref="G7:H13" xr:uid="{C2E51D9C-415E-A840-96CF-42A4AD54C811}"/>
-  <tableColumns count="2">
+<file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{C2E51D9C-415E-A840-96CF-42A4AD54C811}" name="Table915" displayName="Table915" ref="G7:I13" totalsRowShown="0">
+  <autoFilter ref="G7:I13" xr:uid="{C2E51D9C-415E-A840-96CF-42A4AD54C811}"/>
+  <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{5281FA9C-99EC-4D45-889C-8643F65C7BB9}" name="prod_sales"/>
     <tableColumn id="2" xr3:uid="{B556F5FC-DC14-4F40-B8DB-8BBDAC8FDFC1}" name="Column1"/>
+    <tableColumn id="3" xr3:uid="{FA4E6681-908E-5F4C-AB2A-874A62115624}" name="ç"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
-<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{B488AC21-3084-4E7E-AB5D-38898F649B2E}" name="Table8" displayName="Table8" ref="A7:B19" totalsRowShown="0">
   <autoFilter ref="A7:B19" xr:uid="{B488AC21-3084-4E7E-AB5D-38898F649B2E}"/>
   <tableColumns count="2">
@@ -3625,7 +3663,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{955D6FB2-5E71-4F0C-A5B7-63958174CCBB}" name="Table10" displayName="Table10" ref="D21:E23" totalsRowShown="0">
   <autoFilter ref="D21:E23" xr:uid="{955D6FB2-5E71-4F0C-A5B7-63958174CCBB}"/>
   <tableColumns count="2">
@@ -3636,7 +3674,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{EA6E0763-6C65-46EC-8AB8-CB076FF2984B}" name="Table314" displayName="Table314" ref="D7:E19" totalsRowShown="0">
   <autoFilter ref="D7:E19" xr:uid="{EA6E0763-6C65-46EC-8AB8-CB076FF2984B}"/>
   <tableColumns count="2">
@@ -3647,7 +3685,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{E3DDE1CB-D2EC-4895-A1DE-5DAE3B1FA4A0}" name="Table9" displayName="Table9" ref="A21:B27" totalsRowShown="0">
   <autoFilter ref="A21:B27" xr:uid="{E3DDE1CB-D2EC-4895-A1DE-5DAE3B1FA4A0}"/>
   <tableColumns count="2">
@@ -3658,7 +3696,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{EEE1974C-DD2B-4FC1-8231-7E927BDEBBB3}" name="Table15" displayName="Table15" ref="G14:H19" totalsRowShown="0">
   <autoFilter ref="G14:H19" xr:uid="{EEE1974C-DD2B-4FC1-8231-7E927BDEBBB3}"/>
   <tableColumns count="2">
@@ -3669,7 +3707,18 @@
 </table>
 </file>
 
-<file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3CBDE4DA-7C0B-4503-8EDB-ADF0A7222A1A}" name="Table1" displayName="Table1" ref="A12:B17" totalsRowShown="0">
+  <autoFilter ref="A12:B17" xr:uid="{3CBDE4DA-7C0B-4503-8EDB-ADF0A7222A1A}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{6C99A95B-B00D-4300-B101-D3D75563C294}" name="user_login"/>
+    <tableColumn id="2" xr3:uid="{C0FF947C-9527-4405-AB17-B6D40DD8B496}" name="Datatype"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table20.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{AC03ADBA-3354-4069-84CB-68F6242AE90F}" name="Table7" displayName="Table7" ref="A1:Q86" totalsRowShown="0" headerRowDxfId="59" headerRowBorderDxfId="58" tableBorderDxfId="57" totalsRowBorderDxfId="56">
   <autoFilter ref="A1:Q86" xr:uid="{AC03ADBA-3354-4069-84CB-68F6242AE90F}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Q86">
@@ -3698,7 +3747,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table21.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{6758D745-B4E1-4043-A8D2-8D4F7FDE8A08}" name="Table19" displayName="Table19" ref="A1:N95" totalsRowShown="0" headerRowDxfId="38" headerRowBorderDxfId="37" tableBorderDxfId="36" totalsRowBorderDxfId="35">
   <autoFilter ref="A1:N95" xr:uid="{6758D745-B4E1-4043-A8D2-8D4F7FDE8A08}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N85">
@@ -3724,7 +3773,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table22.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="23" xr:uid="{B41F1D88-6BC9-7541-8EAA-179233B1D5E9}" name="Table23" displayName="Table23" ref="A1:E4" totalsRowShown="0" headerRowDxfId="20" headerRowBorderDxfId="19" tableBorderDxfId="18" totalsRowBorderDxfId="17">
   <autoFilter ref="A1:E4" xr:uid="{B41F1D88-6BC9-7541-8EAA-179233B1D5E9}"/>
   <tableColumns count="5">
@@ -3738,18 +3787,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3CBDE4DA-7C0B-4503-8EDB-ADF0A7222A1A}" name="Table1" displayName="Table1" ref="A12:B17" totalsRowShown="0">
-  <autoFilter ref="A12:B17" xr:uid="{3CBDE4DA-7C0B-4503-8EDB-ADF0A7222A1A}"/>
-  <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{6C99A95B-B00D-4300-B101-D3D75563C294}" name="user_login"/>
-    <tableColumn id="2" xr3:uid="{C0FF947C-9527-4405-AB17-B6D40DD8B496}" name="Datatype"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table23.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="24" xr:uid="{E333897C-4734-8E49-9F1A-8F1B50120560}" name="Table24" displayName="Table24" ref="A7:H14" totalsRowShown="0" headerRowDxfId="11" headerRowBorderDxfId="10" tableBorderDxfId="9" totalsRowBorderDxfId="8">
   <autoFilter ref="A7:H14" xr:uid="{E333897C-4734-8E49-9F1A-8F1B50120560}"/>
   <tableColumns count="8">
@@ -3766,7 +3804,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table24.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{32CD3382-E4B9-3F4E-A402-388178C48A05}" name="Table20" displayName="Table20" ref="A5:B10" totalsRowShown="0">
   <autoFilter ref="A5:B10" xr:uid="{32CD3382-E4B9-3F4E-A402-388178C48A05}"/>
   <tableColumns count="2">
@@ -3777,7 +3815,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table25.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{F6FFAADD-2B33-9E40-A7EA-CE1F33C8F6CA}" name="Table21" displayName="Table21" ref="D5:E13" totalsRowShown="0">
   <autoFilter ref="D5:E13" xr:uid="{F6FFAADD-2B33-9E40-A7EA-CE1F33C8F6CA}"/>
   <tableColumns count="2">
@@ -3788,7 +3826,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table26.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{9B4BE8D4-A97F-0745-9A27-A264F92DA22A}" name="Table22" displayName="Table22" ref="G5:H9" totalsRowShown="0">
   <autoFilter ref="G5:H9" xr:uid="{9B4BE8D4-A97F-0745-9A27-A264F92DA22A}"/>
   <tableColumns count="2">
@@ -3866,11 +3904,11 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{EEE9A7FF-A6ED-4209-A1C4-CC197F0AC95C}" name="Table11" displayName="Table11" ref="A7:B15" totalsRowShown="0">
-  <autoFilter ref="A7:B15" xr:uid="{EEE9A7FF-A6ED-4209-A1C4-CC197F0AC95C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{6B7CF076-FA24-B54D-9592-AF69387A5344}" name="Table1119" displayName="Table1119" ref="A9:B17" totalsRowShown="0">
+  <autoFilter ref="A9:B17" xr:uid="{6B7CF076-FA24-B54D-9592-AF69387A5344}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{A70E2D6B-6988-49C6-B102-5D940C03D8A4}" name="invoice"/>
-    <tableColumn id="2" xr3:uid="{4D9C4735-0D32-45DB-B042-737ABFC2EBD5}" name="datatype"/>
+    <tableColumn id="1" xr3:uid="{544EBB55-3AE7-8449-951E-19BAB458A288}" name="invoice"/>
+    <tableColumn id="2" xr3:uid="{687EF95B-432F-6649-A88D-8C791FCDD2A4}" name="datatype"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4179,13 +4217,13 @@
       <selection activeCell="A6" sqref="A6:A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.44140625" customWidth="1"/>
+    <col min="1" max="1" width="12.5" customWidth="1"/>
     <col min="2" max="2" width="74.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4193,7 +4231,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -4201,7 +4239,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -4209,7 +4247,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -4229,28 +4267,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40455DF4-3F31-4947-BCA7-1853A71C76DD}">
   <dimension ref="A1:N95"/>
   <sheetViews>
-    <sheetView topLeftCell="A36" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="I113" sqref="I113"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.77734375" customWidth="1"/>
+    <col min="3" max="3" width="16.83203125" customWidth="1"/>
     <col min="4" max="4" width="12.6640625" customWidth="1"/>
     <col min="5" max="5" width="24.33203125" customWidth="1"/>
-    <col min="6" max="6" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.83203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17.6640625" customWidth="1"/>
-    <col min="8" max="8" width="19.77734375" customWidth="1"/>
-    <col min="9" max="9" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.83203125" customWidth="1"/>
+    <col min="9" max="9" width="14.1640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11" customWidth="1"/>
     <col min="11" max="11" width="20.33203125" customWidth="1"/>
     <col min="12" max="12" width="19" customWidth="1"/>
     <col min="13" max="13" width="16.6640625" customWidth="1"/>
-    <col min="14" max="14" width="16.109375" customWidth="1"/>
+    <col min="14" max="14" width="16.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="25" t="s">
         <v>301</v>
       </c>
@@ -4294,7 +4332,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="28" t="s">
         <v>346</v>
       </c>
@@ -4320,7 +4358,7 @@
       <c r="M2" s="29"/>
       <c r="N2" s="30"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="28" t="s">
         <v>338</v>
       </c>
@@ -4346,7 +4384,7 @@
       <c r="M3" s="29"/>
       <c r="N3" s="30"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="28" t="s">
         <v>339</v>
       </c>
@@ -4372,7 +4410,7 @@
       <c r="M4" s="29"/>
       <c r="N4" s="30"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="28" t="s">
         <v>340</v>
       </c>
@@ -4398,7 +4436,7 @@
       <c r="M5" s="29"/>
       <c r="N5" s="30"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="28" t="s">
         <v>341</v>
       </c>
@@ -4424,7 +4462,7 @@
       <c r="M6" s="29"/>
       <c r="N6" s="30"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="28" t="s">
         <v>342</v>
       </c>
@@ -4450,7 +4488,7 @@
       <c r="M7" s="29"/>
       <c r="N7" s="30"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="28" t="s">
         <v>343</v>
       </c>
@@ -4476,7 +4514,7 @@
       <c r="M8" s="29"/>
       <c r="N8" s="30"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="28" t="s">
         <v>344</v>
       </c>
@@ -4502,7 +4540,7 @@
       <c r="M9" s="29"/>
       <c r="N9" s="30"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="28" t="s">
         <v>345</v>
       </c>
@@ -4528,7 +4566,7 @@
       <c r="M10" s="29"/>
       <c r="N10" s="30"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="28" t="s">
         <v>358</v>
       </c>
@@ -4554,7 +4592,7 @@
       <c r="M11" s="29"/>
       <c r="N11" s="30"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="28" t="s">
         <v>363</v>
       </c>
@@ -4580,7 +4618,7 @@
       <c r="M12" s="29"/>
       <c r="N12" s="30"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="28" t="s">
         <v>309</v>
       </c>
@@ -4606,7 +4644,7 @@
       <c r="M13" s="29"/>
       <c r="N13" s="30"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="28" t="s">
         <v>361</v>
       </c>
@@ -4632,7 +4670,7 @@
       <c r="M14" s="29"/>
       <c r="N14" s="30"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" s="28" t="s">
         <v>362</v>
       </c>
@@ -4658,7 +4696,7 @@
       <c r="M15" s="29"/>
       <c r="N15" s="30"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="28" t="s">
         <v>310</v>
       </c>
@@ -4684,7 +4722,7 @@
       <c r="M16" s="29"/>
       <c r="N16" s="30"/>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" s="28" t="s">
         <v>360</v>
       </c>
@@ -4710,7 +4748,7 @@
       <c r="M17" s="29"/>
       <c r="N17" s="30"/>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" s="28" t="s">
         <v>347</v>
       </c>
@@ -4736,7 +4774,7 @@
       <c r="M18" s="29"/>
       <c r="N18" s="30"/>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" s="28" t="s">
         <v>364</v>
       </c>
@@ -4762,7 +4800,7 @@
       <c r="M19" s="29"/>
       <c r="N19" s="30"/>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" s="28" t="s">
         <v>365</v>
       </c>
@@ -4788,7 +4826,7 @@
       <c r="M20" s="29"/>
       <c r="N20" s="30"/>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" s="28" t="s">
         <v>356</v>
       </c>
@@ -4814,7 +4852,7 @@
       <c r="M21" s="29"/>
       <c r="N21" s="30"/>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" s="28" t="s">
         <v>355</v>
       </c>
@@ -4840,7 +4878,7 @@
       <c r="M22" s="29"/>
       <c r="N22" s="30"/>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" s="28" t="s">
         <v>357</v>
       </c>
@@ -4866,7 +4904,7 @@
       <c r="M23" s="29"/>
       <c r="N23" s="30"/>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24" s="28" t="s">
         <v>367</v>
       </c>
@@ -4892,7 +4930,7 @@
       <c r="M24" s="29"/>
       <c r="N24" s="30"/>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25" s="28" t="s">
         <v>368</v>
       </c>
@@ -4918,7 +4956,7 @@
       <c r="M25" s="29"/>
       <c r="N25" s="30"/>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26" s="28" t="s">
         <v>359</v>
       </c>
@@ -4944,7 +4982,7 @@
       <c r="M26" s="29"/>
       <c r="N26" s="30"/>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" s="28" t="s">
         <v>366</v>
       </c>
@@ -4970,7 +5008,7 @@
       <c r="M27" s="29"/>
       <c r="N27" s="30"/>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28" s="28" t="s">
         <v>369</v>
       </c>
@@ -4996,7 +5034,7 @@
       <c r="M28" s="29"/>
       <c r="N28" s="30"/>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A29" s="28" t="s">
         <v>370</v>
       </c>
@@ -5022,7 +5060,7 @@
       <c r="M29" s="29"/>
       <c r="N29" s="30"/>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A30" s="28" t="s">
         <v>376</v>
       </c>
@@ -5048,7 +5086,7 @@
       <c r="M30" s="29"/>
       <c r="N30" s="30"/>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A31" s="28" t="s">
         <v>377</v>
       </c>
@@ -5074,7 +5112,7 @@
       <c r="M31" s="29"/>
       <c r="N31" s="30"/>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A32" s="28" t="s">
         <v>378</v>
       </c>
@@ -5100,7 +5138,7 @@
       <c r="M32" s="29"/>
       <c r="N32" s="30"/>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A33" s="28" t="s">
         <v>379</v>
       </c>
@@ -5126,7 +5164,7 @@
       <c r="M33" s="29"/>
       <c r="N33" s="30"/>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A34" s="28" t="s">
         <v>380</v>
       </c>
@@ -5152,7 +5190,7 @@
       <c r="M34" s="29"/>
       <c r="N34" s="30"/>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A35" s="28" t="s">
         <v>381</v>
       </c>
@@ -5178,7 +5216,7 @@
       <c r="M35" s="29"/>
       <c r="N35" s="30"/>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A36" s="28" t="s">
         <v>382</v>
       </c>
@@ -5204,7 +5242,7 @@
       <c r="M36" s="29"/>
       <c r="N36" s="30"/>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A37" s="28" t="s">
         <v>371</v>
       </c>
@@ -5230,7 +5268,7 @@
       <c r="M37" s="29"/>
       <c r="N37" s="30"/>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A38" s="28" t="s">
         <v>372</v>
       </c>
@@ -5256,7 +5294,7 @@
       <c r="M38" s="29"/>
       <c r="N38" s="30"/>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A39" s="28" t="s">
         <v>373</v>
       </c>
@@ -5282,7 +5320,7 @@
       <c r="M39" s="29"/>
       <c r="N39" s="30"/>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A40" s="28" t="s">
         <v>374</v>
       </c>
@@ -5308,7 +5346,7 @@
       <c r="M40" s="29"/>
       <c r="N40" s="30"/>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A41" s="28" t="s">
         <v>384</v>
       </c>
@@ -5334,7 +5372,7 @@
       <c r="M41" s="29"/>
       <c r="N41" s="30"/>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A42" s="28" t="s">
         <v>383</v>
       </c>
@@ -5360,7 +5398,7 @@
       <c r="M42" s="29"/>
       <c r="N42" s="30"/>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A43" s="28" t="s">
         <v>385</v>
       </c>
@@ -5386,7 +5424,7 @@
       <c r="M43" s="29"/>
       <c r="N43" s="30"/>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A44" s="28" t="s">
         <v>330</v>
       </c>
@@ -5412,7 +5450,7 @@
       <c r="M44" s="29"/>
       <c r="N44" s="30"/>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A45" s="28" t="s">
         <v>329</v>
       </c>
@@ -5438,7 +5476,7 @@
       <c r="M45" s="29"/>
       <c r="N45" s="30"/>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A46" s="28" t="s">
         <v>313</v>
       </c>
@@ -5464,7 +5502,7 @@
       <c r="M46" s="29"/>
       <c r="N46" s="30"/>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A47" s="28" t="s">
         <v>314</v>
       </c>
@@ -5490,7 +5528,7 @@
       <c r="M47" s="29"/>
       <c r="N47" s="30"/>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A48" s="28" t="s">
         <v>332</v>
       </c>
@@ -5516,7 +5554,7 @@
       <c r="M48" s="29"/>
       <c r="N48" s="30"/>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A49" s="28" t="s">
         <v>316</v>
       </c>
@@ -5542,7 +5580,7 @@
       <c r="M49" s="29"/>
       <c r="N49" s="30"/>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A50" s="28" t="s">
         <v>320</v>
       </c>
@@ -5568,7 +5606,7 @@
       <c r="M50" s="29"/>
       <c r="N50" s="30"/>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A51" s="28" t="s">
         <v>305</v>
       </c>
@@ -5594,7 +5632,7 @@
       <c r="M51" s="29"/>
       <c r="N51" s="30"/>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A52" s="28" t="s">
         <v>308</v>
       </c>
@@ -5620,7 +5658,7 @@
       <c r="M52" s="29"/>
       <c r="N52" s="30"/>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A53" s="28" t="s">
         <v>331</v>
       </c>
@@ -5646,7 +5684,7 @@
       <c r="M53" s="29"/>
       <c r="N53" s="30"/>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A54" s="28" t="s">
         <v>322</v>
       </c>
@@ -5672,7 +5710,7 @@
       <c r="M54" s="29"/>
       <c r="N54" s="30"/>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A55" s="28" t="s">
         <v>349</v>
       </c>
@@ -5698,7 +5736,7 @@
       <c r="M55" s="29"/>
       <c r="N55" s="30"/>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A56" s="28" t="s">
         <v>350</v>
       </c>
@@ -5724,7 +5762,7 @@
       <c r="M56" s="29"/>
       <c r="N56" s="30"/>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A57" s="28" t="s">
         <v>351</v>
       </c>
@@ -5750,7 +5788,7 @@
       <c r="M57" s="29"/>
       <c r="N57" s="30"/>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A58" s="28" t="s">
         <v>352</v>
       </c>
@@ -5776,7 +5814,7 @@
       <c r="M58" s="29"/>
       <c r="N58" s="30"/>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A59" s="28" t="s">
         <v>353</v>
       </c>
@@ -5802,7 +5840,7 @@
       <c r="M59" s="29"/>
       <c r="N59" s="30"/>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A60" s="28" t="s">
         <v>354</v>
       </c>
@@ -5828,7 +5866,7 @@
       <c r="M60" s="29"/>
       <c r="N60" s="30"/>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A61" s="28" t="s">
         <v>333</v>
       </c>
@@ -5854,7 +5892,7 @@
       <c r="M61" s="29"/>
       <c r="N61" s="30"/>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A62" s="28" t="s">
         <v>334</v>
       </c>
@@ -5880,7 +5918,7 @@
       <c r="M62" s="29"/>
       <c r="N62" s="30"/>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A63" s="28" t="s">
         <v>335</v>
       </c>
@@ -5906,7 +5944,7 @@
       <c r="M63" s="29"/>
       <c r="N63" s="30"/>
     </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A64" s="28" t="s">
         <v>336</v>
       </c>
@@ -5932,7 +5970,7 @@
       <c r="M64" s="29"/>
       <c r="N64" s="30"/>
     </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A65" s="28" t="s">
         <v>337</v>
       </c>
@@ -5958,7 +5996,7 @@
       <c r="M65" s="29"/>
       <c r="N65" s="30"/>
     </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A66" s="28" t="s">
         <v>315</v>
       </c>
@@ -5984,7 +6022,7 @@
       <c r="M66" s="29"/>
       <c r="N66" s="30"/>
     </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A67" s="28" t="s">
         <v>328</v>
       </c>
@@ -6010,7 +6048,7 @@
       <c r="M67" s="29"/>
       <c r="N67" s="30"/>
     </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A68" s="28" t="s">
         <v>327</v>
       </c>
@@ -6036,7 +6074,7 @@
       <c r="M68" s="29"/>
       <c r="N68" s="30"/>
     </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A69" s="28" t="s">
         <v>318</v>
       </c>
@@ -6062,7 +6100,7 @@
       <c r="M69" s="29"/>
       <c r="N69" s="30"/>
     </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A70" s="28" t="s">
         <v>318</v>
       </c>
@@ -6088,7 +6126,7 @@
       <c r="M70" s="29"/>
       <c r="N70" s="30"/>
     </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A71" s="28" t="s">
         <v>324</v>
       </c>
@@ -6114,7 +6152,7 @@
       <c r="M71" s="29"/>
       <c r="N71" s="30"/>
     </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A72" s="28" t="s">
         <v>306</v>
       </c>
@@ -6140,7 +6178,7 @@
       <c r="M72" s="29"/>
       <c r="N72" s="30"/>
     </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A73" s="28" t="s">
         <v>307</v>
       </c>
@@ -6166,7 +6204,7 @@
       <c r="M73" s="29"/>
       <c r="N73" s="30"/>
     </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A74" s="28" t="s">
         <v>326</v>
       </c>
@@ -6192,7 +6230,7 @@
       <c r="M74" s="29"/>
       <c r="N74" s="30"/>
     </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A75" s="28" t="s">
         <v>311</v>
       </c>
@@ -6218,7 +6256,7 @@
       <c r="M75" s="29"/>
       <c r="N75" s="30"/>
     </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A76" s="28" t="s">
         <v>311</v>
       </c>
@@ -6244,7 +6282,7 @@
       <c r="M76" s="29"/>
       <c r="N76" s="30"/>
     </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A77" s="28" t="s">
         <v>312</v>
       </c>
@@ -6270,7 +6308,7 @@
       <c r="M77" s="29"/>
       <c r="N77" s="30"/>
     </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A78" s="28" t="s">
         <v>323</v>
       </c>
@@ -6296,7 +6334,7 @@
       <c r="M78" s="29"/>
       <c r="N78" s="30"/>
     </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A79" s="28" t="s">
         <v>319</v>
       </c>
@@ -6322,7 +6360,7 @@
       <c r="M79" s="29"/>
       <c r="N79" s="30"/>
     </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A80" s="28" t="s">
         <v>317</v>
       </c>
@@ -6348,7 +6386,7 @@
       <c r="M80" s="29"/>
       <c r="N80" s="30"/>
     </row>
-    <row r="81" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A81" s="28" t="s">
         <v>321</v>
       </c>
@@ -6374,7 +6412,7 @@
       <c r="M81" s="29"/>
       <c r="N81" s="30"/>
     </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A82" s="28" t="s">
         <v>386</v>
       </c>
@@ -6400,7 +6438,7 @@
       <c r="M82" s="29"/>
       <c r="N82" s="30"/>
     </row>
-    <row r="83" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A83" s="28" t="s">
         <v>387</v>
       </c>
@@ -6426,7 +6464,7 @@
       <c r="M83" s="29"/>
       <c r="N83" s="30"/>
     </row>
-    <row r="84" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A84" s="28" t="s">
         <v>388</v>
       </c>
@@ -6452,7 +6490,7 @@
       <c r="M84" s="29"/>
       <c r="N84" s="30"/>
     </row>
-    <row r="85" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A85" s="31"/>
       <c r="B85" s="32"/>
       <c r="C85" s="32"/>
@@ -6468,7 +6506,7 @@
       <c r="M85" s="32"/>
       <c r="N85" s="33"/>
     </row>
-    <row r="86" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A86" s="31"/>
       <c r="B86" s="32" t="s">
         <v>389</v>
@@ -6488,7 +6526,7 @@
       <c r="M86" s="32"/>
       <c r="N86" s="33"/>
     </row>
-    <row r="87" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A87" s="31"/>
       <c r="B87" s="32" t="s">
         <v>390</v>
@@ -6508,7 +6546,7 @@
       <c r="M87" s="32"/>
       <c r="N87" s="33"/>
     </row>
-    <row r="88" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A88" s="31"/>
       <c r="B88" s="32" t="s">
         <v>391</v>
@@ -6528,7 +6566,7 @@
       <c r="M88" s="32"/>
       <c r="N88" s="33"/>
     </row>
-    <row r="89" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A89" s="31"/>
       <c r="B89" s="32" t="s">
         <v>392</v>
@@ -6548,7 +6586,7 @@
       <c r="M89" s="32"/>
       <c r="N89" s="33"/>
     </row>
-    <row r="90" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A90" s="31"/>
       <c r="B90" s="32" t="s">
         <v>393</v>
@@ -6568,7 +6606,7 @@
       <c r="M90" s="32"/>
       <c r="N90" s="33"/>
     </row>
-    <row r="91" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A91" s="31"/>
       <c r="B91" s="32" t="s">
         <v>394</v>
@@ -6588,7 +6626,7 @@
       <c r="M91" s="32"/>
       <c r="N91" s="33"/>
     </row>
-    <row r="92" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A92" s="31"/>
       <c r="B92" s="32" t="s">
         <v>395</v>
@@ -6608,7 +6646,7 @@
       <c r="M92" s="32"/>
       <c r="N92" s="33"/>
     </row>
-    <row r="93" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A93" s="31"/>
       <c r="B93" s="32" t="s">
         <v>396</v>
@@ -6628,7 +6666,7 @@
       <c r="M93" s="32"/>
       <c r="N93" s="33"/>
     </row>
-    <row r="94" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A94" s="31"/>
       <c r="B94" s="32" t="s">
         <v>397</v>
@@ -6648,7 +6686,7 @@
       <c r="M94" s="32"/>
       <c r="N94" s="33"/>
     </row>
-    <row r="95" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A95" s="31"/>
       <c r="B95" s="32" t="s">
         <v>398</v>
@@ -6685,17 +6723,17 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.44140625" customWidth="1"/>
+    <col min="1" max="1" width="16.5" customWidth="1"/>
     <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.109375" customWidth="1"/>
+    <col min="3" max="3" width="14.1640625" customWidth="1"/>
     <col min="4" max="4" width="16.6640625" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
-    <col min="6" max="6" width="18.109375" customWidth="1"/>
+    <col min="6" max="6" width="18.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="25" t="s">
         <v>403</v>
       </c>
@@ -6712,7 +6750,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="28">
         <v>1</v>
       </c>
@@ -6727,7 +6765,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="28">
         <v>2</v>
       </c>
@@ -6742,7 +6780,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="31">
         <v>3</v>
       </c>
@@ -6757,7 +6795,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="25" t="s">
         <v>407</v>
       </c>
@@ -6783,7 +6821,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="28">
         <v>1</v>
       </c>
@@ -6803,7 +6841,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="28">
         <v>2</v>
       </c>
@@ -6823,7 +6861,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="28">
         <v>3</v>
       </c>
@@ -6843,7 +6881,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="28">
         <v>4</v>
       </c>
@@ -6863,7 +6901,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="28">
         <v>5</v>
       </c>
@@ -6883,7 +6921,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="28">
         <v>6</v>
       </c>
@@ -6903,7 +6941,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="31">
         <v>7</v>
       </c>
@@ -6940,37 +6978,37 @@
       <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.77734375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="43" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" s="56" t="s">
         <v>298</v>
       </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="45"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="46"/>
-      <c r="B2" s="47"/>
-      <c r="C2" s="47"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="48"/>
-    </row>
-    <row r="3" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="49"/>
-      <c r="B3" s="50"/>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
-      <c r="E3" s="51"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="58"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="59"/>
+      <c r="B2" s="60"/>
+      <c r="C2" s="60"/>
+      <c r="D2" s="60"/>
+      <c r="E2" s="61"/>
+    </row>
+    <row r="3" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="62"/>
+      <c r="B3" s="63"/>
+      <c r="C3" s="63"/>
+      <c r="D3" s="63"/>
+      <c r="E3" s="64"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>400</v>
       </c>
@@ -6993,7 +7031,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="20" t="s">
         <v>403</v>
       </c>
@@ -7013,7 +7051,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="20" t="s">
         <v>91</v>
       </c>
@@ -7030,7 +7068,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>406</v>
       </c>
@@ -7047,7 +7085,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>404</v>
       </c>
@@ -7064,7 +7102,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>405</v>
       </c>
@@ -7078,7 +7116,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="D11" t="s">
         <v>412</v>
       </c>
@@ -7086,7 +7124,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="D12" t="s">
         <v>432</v>
       </c>
@@ -7094,7 +7132,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="D13" t="s">
         <v>433</v>
       </c>
@@ -7119,92 +7157,92 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="F44" sqref="F44"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.109375" customWidth="1"/>
-    <col min="2" max="2" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.109375" customWidth="1"/>
-    <col min="5" max="5" width="23.77734375" customWidth="1"/>
+    <col min="1" max="1" width="22.1640625" customWidth="1"/>
+    <col min="2" max="2" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.1640625" customWidth="1"/>
+    <col min="5" max="5" width="23.83203125" customWidth="1"/>
     <col min="6" max="6" width="17.6640625" customWidth="1"/>
     <col min="7" max="7" width="22.33203125" customWidth="1"/>
-    <col min="8" max="8" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="43" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" s="56" t="s">
         <v>294</v>
       </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="45"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="46"/>
-      <c r="B2" s="47"/>
-      <c r="C2" s="47"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="48"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="46"/>
-      <c r="B3" s="47"/>
-      <c r="C3" s="47"/>
-      <c r="D3" s="47"/>
-      <c r="E3" s="48"/>
-    </row>
-    <row r="4" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="49"/>
-      <c r="B4" s="50"/>
-      <c r="C4" s="50"/>
-      <c r="D4" s="50"/>
-      <c r="E4" s="51"/>
-    </row>
-    <row r="5" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="43" t="s">
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="58"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="59"/>
+      <c r="B2" s="60"/>
+      <c r="C2" s="60"/>
+      <c r="D2" s="60"/>
+      <c r="E2" s="61"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="59"/>
+      <c r="B3" s="60"/>
+      <c r="C3" s="60"/>
+      <c r="D3" s="60"/>
+      <c r="E3" s="61"/>
+    </row>
+    <row r="4" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="62"/>
+      <c r="B4" s="63"/>
+      <c r="C4" s="63"/>
+      <c r="D4" s="63"/>
+      <c r="E4" s="64"/>
+    </row>
+    <row r="5" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="56" t="s">
         <v>295</v>
       </c>
-      <c r="B6" s="52"/>
-      <c r="C6" s="52"/>
-      <c r="D6" s="52"/>
-      <c r="E6" s="53"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="54"/>
-      <c r="B7" s="55"/>
-      <c r="C7" s="55"/>
-      <c r="D7" s="55"/>
-      <c r="E7" s="56"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="54"/>
-      <c r="B8" s="55"/>
-      <c r="C8" s="55"/>
-      <c r="D8" s="55"/>
-      <c r="E8" s="56"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="54"/>
-      <c r="B9" s="55"/>
-      <c r="C9" s="55"/>
-      <c r="D9" s="55"/>
-      <c r="E9" s="56"/>
-    </row>
-    <row r="10" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="57"/>
-      <c r="B10" s="58"/>
-      <c r="C10" s="58"/>
-      <c r="D10" s="58"/>
-      <c r="E10" s="59"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B6" s="65"/>
+      <c r="C6" s="65"/>
+      <c r="D6" s="65"/>
+      <c r="E6" s="66"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="67"/>
+      <c r="B7" s="68"/>
+      <c r="C7" s="68"/>
+      <c r="D7" s="68"/>
+      <c r="E7" s="69"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="67"/>
+      <c r="B8" s="68"/>
+      <c r="C8" s="68"/>
+      <c r="D8" s="68"/>
+      <c r="E8" s="69"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="67"/>
+      <c r="B9" s="68"/>
+      <c r="C9" s="68"/>
+      <c r="D9" s="68"/>
+      <c r="E9" s="69"/>
+    </row>
+    <row r="10" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="70"/>
+      <c r="B10" s="71"/>
+      <c r="C10" s="71"/>
+      <c r="D10" s="71"/>
+      <c r="E10" s="72"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -7224,7 +7262,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="20" t="s">
         <v>12</v>
       </c>
@@ -7244,7 +7282,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>18</v>
       </c>
@@ -7264,7 +7302,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>21</v>
       </c>
@@ -7284,7 +7322,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>24</v>
       </c>
@@ -7298,7 +7336,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>27</v>
       </c>
@@ -7312,7 +7350,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D18" t="s">
         <v>28</v>
       </c>
@@ -7320,7 +7358,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>30</v>
       </c>
@@ -7334,7 +7372,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="20" t="s">
         <v>32</v>
       </c>
@@ -7348,7 +7386,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>18</v>
       </c>
@@ -7362,7 +7400,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -7376,7 +7414,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>27</v>
       </c>
@@ -7390,7 +7428,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D24" t="s">
         <v>36</v>
       </c>
@@ -7398,7 +7436,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>38</v>
       </c>
@@ -7412,7 +7450,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="20" t="s">
         <v>39</v>
       </c>
@@ -7420,7 +7458,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="20" t="s">
         <v>32</v>
       </c>
@@ -7434,7 +7472,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>22</v>
       </c>
@@ -7448,7 +7486,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>26</v>
       </c>
@@ -7462,7 +7500,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>28</v>
       </c>
@@ -7470,7 +7508,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="20" t="s">
         <v>41</v>
       </c>
@@ -7478,7 +7516,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" s="38" t="s">
         <v>444</v>
       </c>
@@ -7489,7 +7527,7 @@
       <c r="F36" s="38"/>
       <c r="G36" s="38"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="39"/>
       <c r="B37" s="39"/>
       <c r="C37" s="39"/>
@@ -7498,7 +7536,7 @@
       <c r="F37" s="39"/>
       <c r="G37" s="39"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" s="40" t="s">
         <v>2</v>
       </c>
@@ -7509,15 +7547,15 @@
         <v>445</v>
       </c>
       <c r="D38" s="39"/>
-      <c r="E38" s="66" t="s">
+      <c r="E38" s="49" t="s">
         <v>456</v>
       </c>
-      <c r="F38" s="66" t="s">
+      <c r="F38" s="49" t="s">
         <v>457</v>
       </c>
-      <c r="G38" s="63"/>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G38" s="46"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" s="41" t="s">
         <v>461</v>
       </c>
@@ -7528,15 +7566,15 @@
         <v>446</v>
       </c>
       <c r="D39" s="39"/>
-      <c r="E39" s="67">
+      <c r="E39" s="50">
         <v>5</v>
       </c>
-      <c r="F39" s="67" t="s">
+      <c r="F39" s="50" t="s">
         <v>458</v>
       </c>
-      <c r="G39" s="61"/>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G39" s="44"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" s="39" t="s">
         <v>447</v>
       </c>
@@ -7547,15 +7585,15 @@
         <v>446</v>
       </c>
       <c r="D40" s="39"/>
-      <c r="E40" s="68">
+      <c r="E40" s="51">
         <v>4</v>
       </c>
-      <c r="F40" s="68" t="s">
+      <c r="F40" s="51" t="s">
         <v>459</v>
       </c>
-      <c r="G40" s="61"/>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G40" s="44"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" s="41" t="s">
         <v>449</v>
       </c>
@@ -7566,15 +7604,15 @@
         <v>446</v>
       </c>
       <c r="D41" s="39"/>
-      <c r="E41" s="69">
+      <c r="E41" s="52">
         <v>3</v>
       </c>
-      <c r="F41" s="69" t="s">
+      <c r="F41" s="52" t="s">
         <v>463</v>
       </c>
-      <c r="G41" s="61"/>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G41" s="44"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" s="39" t="s">
         <v>460</v>
       </c>
@@ -7585,15 +7623,15 @@
         <v>1</v>
       </c>
       <c r="D42" s="39"/>
-      <c r="E42" s="70">
+      <c r="E42" s="53">
         <v>2</v>
       </c>
-      <c r="F42" s="70" t="s">
+      <c r="F42" s="53" t="s">
         <v>464</v>
       </c>
       <c r="G42" s="42"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" s="39" t="s">
         <v>27</v>
       </c>
@@ -7604,28 +7642,28 @@
         <v>446</v>
       </c>
       <c r="D43" s="39"/>
-      <c r="E43" s="71">
+      <c r="E43" s="54">
         <v>1</v>
       </c>
-      <c r="F43" s="71" t="s">
+      <c r="F43" s="54" t="s">
         <v>465</v>
       </c>
       <c r="G43" s="39"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" s="39"/>
       <c r="B44" s="39"/>
       <c r="C44" s="39"/>
       <c r="D44" s="39"/>
-      <c r="E44" s="72">
+      <c r="E44" s="55">
         <v>0</v>
       </c>
-      <c r="F44" s="72" t="s">
+      <c r="F44" s="55" t="s">
         <v>466</v>
       </c>
       <c r="G44" s="39"/>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" s="39"/>
       <c r="B45" s="39"/>
       <c r="C45" s="39"/>
@@ -7634,7 +7672,7 @@
       <c r="F45" s="39"/>
       <c r="G45" s="39"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" s="39"/>
       <c r="B46" s="39"/>
       <c r="C46" s="39"/>
@@ -7643,7 +7681,7 @@
       <c r="F46" s="39"/>
       <c r="G46" s="39"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" s="40" t="s">
         <v>9</v>
       </c>
@@ -7654,11 +7692,11 @@
         <v>445</v>
       </c>
       <c r="D47" s="39"/>
-      <c r="E47" s="63"/>
-      <c r="F47" s="63"/>
-      <c r="G47" s="63"/>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E47" s="46"/>
+      <c r="F47" s="46"/>
+      <c r="G47" s="46"/>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" s="41" t="s">
         <v>462</v>
       </c>
@@ -7669,11 +7707,11 @@
         <v>446</v>
       </c>
       <c r="D48" s="39"/>
-      <c r="E48" s="61"/>
-      <c r="F48" s="61"/>
-      <c r="G48" s="61"/>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E48" s="44"/>
+      <c r="F48" s="44"/>
+      <c r="G48" s="44"/>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" s="39" t="s">
         <v>91</v>
       </c>
@@ -7684,11 +7722,11 @@
         <v>446</v>
       </c>
       <c r="D49" s="39"/>
-      <c r="E49" s="61"/>
-      <c r="F49" s="61"/>
-      <c r="G49" s="61"/>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E49" s="44"/>
+      <c r="F49" s="44"/>
+      <c r="G49" s="44"/>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" s="41" t="s">
         <v>450</v>
       </c>
@@ -7699,11 +7737,11 @@
         <v>446</v>
       </c>
       <c r="D50" s="39"/>
-      <c r="E50" s="61"/>
-      <c r="F50" s="61"/>
-      <c r="G50" s="61"/>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E50" s="44"/>
+      <c r="F50" s="44"/>
+      <c r="G50" s="44"/>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" s="39" t="s">
         <v>452</v>
       </c>
@@ -7714,11 +7752,11 @@
         <v>446</v>
       </c>
       <c r="D51" s="39"/>
-      <c r="E51" s="61"/>
-      <c r="F51" s="61"/>
-      <c r="G51" s="61"/>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E51" s="44"/>
+      <c r="F51" s="44"/>
+      <c r="G51" s="44"/>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" s="41" t="s">
         <v>453</v>
       </c>
@@ -7729,11 +7767,11 @@
         <v>446</v>
       </c>
       <c r="D52" s="39"/>
-      <c r="E52" s="61"/>
-      <c r="F52" s="61"/>
-      <c r="G52" s="61"/>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E52" s="44"/>
+      <c r="F52" s="44"/>
+      <c r="G52" s="44"/>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" s="39" t="s">
         <v>29</v>
       </c>
@@ -7744,11 +7782,11 @@
         <v>446</v>
       </c>
       <c r="D53" s="39"/>
-      <c r="E53" s="61"/>
-      <c r="F53" s="61"/>
-      <c r="G53" s="61"/>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E53" s="44"/>
+      <c r="F53" s="44"/>
+      <c r="G53" s="44"/>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" s="41" t="s">
         <v>31</v>
       </c>
@@ -7759,11 +7797,11 @@
         <v>446</v>
       </c>
       <c r="D54" s="39"/>
-      <c r="E54" s="61"/>
-      <c r="F54" s="61"/>
-      <c r="G54" s="61"/>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E54" s="44"/>
+      <c r="F54" s="44"/>
+      <c r="G54" s="44"/>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" s="39" t="s">
         <v>33</v>
       </c>
@@ -7774,11 +7812,11 @@
         <v>446</v>
       </c>
       <c r="D55" s="39"/>
-      <c r="E55" s="61"/>
-      <c r="F55" s="61"/>
-      <c r="G55" s="61"/>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E55" s="44"/>
+      <c r="F55" s="44"/>
+      <c r="G55" s="44"/>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" s="41" t="s">
         <v>34</v>
       </c>
@@ -7789,11 +7827,11 @@
         <v>446</v>
       </c>
       <c r="D56" s="39"/>
-      <c r="E56" s="61"/>
-      <c r="F56" s="61"/>
-      <c r="G56" s="61"/>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E56" s="44"/>
+      <c r="F56" s="44"/>
+      <c r="G56" s="44"/>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" s="39" t="s">
         <v>35</v>
       </c>
@@ -7804,11 +7842,11 @@
         <v>446</v>
       </c>
       <c r="D57" s="39"/>
-      <c r="E57" s="61"/>
-      <c r="F57" s="61"/>
-      <c r="G57" s="61"/>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E57" s="44"/>
+      <c r="F57" s="44"/>
+      <c r="G57" s="44"/>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" s="41" t="s">
         <v>454</v>
       </c>
@@ -7819,11 +7857,11 @@
         <v>446</v>
       </c>
       <c r="D58" s="39"/>
-      <c r="E58" s="61"/>
-      <c r="F58" s="61"/>
-      <c r="G58" s="61"/>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E58" s="44"/>
+      <c r="F58" s="44"/>
+      <c r="G58" s="44"/>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" s="39" t="s">
         <v>455</v>
       </c>
@@ -7834,11 +7872,11 @@
         <v>446</v>
       </c>
       <c r="D59" s="39"/>
-      <c r="E59" s="61"/>
-      <c r="F59" s="61"/>
-      <c r="G59" s="61"/>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E59" s="44"/>
+      <c r="F59" s="44"/>
+      <c r="G59" s="44"/>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" s="41" t="s">
         <v>37</v>
       </c>
@@ -7849,20 +7887,20 @@
         <v>446</v>
       </c>
       <c r="D60" s="39"/>
-      <c r="E60" s="61"/>
-      <c r="F60" s="61"/>
-      <c r="G60" s="61"/>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A61" s="60"/>
-      <c r="B61" s="61"/>
-      <c r="C61" s="62"/>
-      <c r="D61" s="61"/>
-      <c r="E61" s="60"/>
-      <c r="F61" s="61"/>
-      <c r="G61" s="62"/>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E60" s="44"/>
+      <c r="F60" s="44"/>
+      <c r="G60" s="44"/>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A61" s="43"/>
+      <c r="B61" s="44"/>
+      <c r="C61" s="45"/>
+      <c r="D61" s="44"/>
+      <c r="E61" s="43"/>
+      <c r="F61" s="44"/>
+      <c r="G61" s="45"/>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62" s="39"/>
       <c r="B62" s="39"/>
       <c r="C62" s="39"/>
@@ -7871,73 +7909,73 @@
       <c r="F62" s="39"/>
       <c r="G62" s="39"/>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A63" s="65"/>
-      <c r="B63" s="65"/>
-      <c r="C63" s="64"/>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A63" s="48"/>
+      <c r="B63" s="48"/>
+      <c r="C63" s="47"/>
       <c r="D63" s="39"/>
       <c r="E63" s="39"/>
       <c r="F63" s="39"/>
       <c r="G63" s="39"/>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A64" s="65"/>
-      <c r="B64" s="65"/>
-      <c r="C64" s="64"/>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A64" s="48"/>
+      <c r="B64" s="48"/>
+      <c r="C64" s="47"/>
       <c r="D64" s="39"/>
       <c r="E64" s="39"/>
       <c r="F64" s="39"/>
       <c r="G64" s="39"/>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A65" s="65"/>
-      <c r="B65" s="65"/>
-      <c r="C65" s="64"/>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A65" s="48"/>
+      <c r="B65" s="48"/>
+      <c r="C65" s="47"/>
       <c r="D65" s="39"/>
       <c r="E65" s="39"/>
       <c r="F65" s="39"/>
       <c r="G65" s="39"/>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A66" s="65"/>
-      <c r="B66" s="65"/>
-      <c r="C66" s="64"/>
-      <c r="D66" s="64"/>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A66" s="48"/>
+      <c r="B66" s="48"/>
+      <c r="C66" s="47"/>
+      <c r="D66" s="47"/>
       <c r="E66" s="39"/>
       <c r="F66" s="39"/>
       <c r="G66" s="39"/>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A67" s="65"/>
-      <c r="B67" s="65"/>
-      <c r="C67" s="64"/>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A67" s="48"/>
+      <c r="B67" s="48"/>
+      <c r="C67" s="47"/>
       <c r="D67" s="39"/>
       <c r="E67" s="39"/>
       <c r="F67" s="39"/>
       <c r="G67" s="39"/>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A68" s="65"/>
-      <c r="B68" s="65"/>
-      <c r="C68" s="64"/>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A68" s="48"/>
+      <c r="B68" s="48"/>
+      <c r="C68" s="47"/>
       <c r="D68" s="39"/>
       <c r="E68" s="39"/>
       <c r="F68" s="39"/>
       <c r="G68" s="39"/>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A69" s="65"/>
-      <c r="B69" s="65"/>
-      <c r="C69" s="64"/>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A69" s="48"/>
+      <c r="B69" s="48"/>
+      <c r="C69" s="47"/>
       <c r="D69" s="39"/>
       <c r="E69" s="39"/>
       <c r="F69" s="39"/>
       <c r="G69" s="39"/>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A70" s="64"/>
-      <c r="B70" s="64"/>
-      <c r="C70" s="64"/>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A70" s="47"/>
+      <c r="B70" s="47"/>
+      <c r="C70" s="47"/>
       <c r="D70" s="39"/>
       <c r="E70" s="39"/>
       <c r="F70" s="39"/>
@@ -7970,55 +8008,55 @@
       <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="43" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="56" t="s">
         <v>292</v>
       </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="45"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="46"/>
-      <c r="B2" s="47"/>
-      <c r="C2" s="47"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
-      <c r="F2" s="48"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="46"/>
-      <c r="B3" s="47"/>
-      <c r="C3" s="47"/>
-      <c r="D3" s="47"/>
-      <c r="E3" s="47"/>
-      <c r="F3" s="48"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="46"/>
-      <c r="B4" s="47"/>
-      <c r="C4" s="47"/>
-      <c r="D4" s="47"/>
-      <c r="E4" s="47"/>
-      <c r="F4" s="48"/>
-    </row>
-    <row r="5" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="49"/>
-      <c r="B5" s="50"/>
-      <c r="C5" s="50"/>
-      <c r="D5" s="50"/>
-      <c r="E5" s="50"/>
-      <c r="F5" s="51"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="58"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="59"/>
+      <c r="B2" s="60"/>
+      <c r="C2" s="60"/>
+      <c r="D2" s="60"/>
+      <c r="E2" s="60"/>
+      <c r="F2" s="61"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="59"/>
+      <c r="B3" s="60"/>
+      <c r="C3" s="60"/>
+      <c r="D3" s="60"/>
+      <c r="E3" s="60"/>
+      <c r="F3" s="61"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="59"/>
+      <c r="B4" s="60"/>
+      <c r="C4" s="60"/>
+      <c r="D4" s="60"/>
+      <c r="E4" s="60"/>
+      <c r="F4" s="61"/>
+    </row>
+    <row r="5" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="62"/>
+      <c r="B5" s="63"/>
+      <c r="C5" s="63"/>
+      <c r="D5" s="63"/>
+      <c r="E5" s="63"/>
+      <c r="F5" s="64"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="18"/>
       <c r="B6" s="18"/>
       <c r="C6" s="18"/>
@@ -8026,7 +8064,7 @@
       <c r="E6" s="18"/>
       <c r="F6" s="18"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -8037,7 +8075,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="20" t="s">
         <v>45</v>
       </c>
@@ -8048,7 +8086,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>47</v>
       </c>
@@ -8059,7 +8097,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>29</v>
       </c>
@@ -8070,7 +8108,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>31</v>
       </c>
@@ -8081,7 +8119,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>33</v>
       </c>
@@ -8092,7 +8130,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>34</v>
       </c>
@@ -8100,7 +8138,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>35</v>
       </c>
@@ -8108,7 +8146,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>52</v>
       </c>
@@ -8116,7 +8154,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>53</v>
       </c>
@@ -8124,7 +8162,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>54</v>
       </c>
@@ -8132,7 +8170,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>55</v>
       </c>
@@ -8140,7 +8178,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>56</v>
       </c>
@@ -8161,132 +8199,251 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8FAEA09-6CEA-024D-AB54-2470DDA2FDE1}">
-  <dimension ref="A1:I25"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="43" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" s="56" t="s">
         <v>290</v>
       </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
-      <c r="I1" s="45"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="46"/>
-      <c r="B2" s="47"/>
-      <c r="C2" s="47"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
-      <c r="F2" s="47"/>
-      <c r="G2" s="47"/>
-      <c r="H2" s="47"/>
-      <c r="I2" s="48"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="46"/>
-      <c r="B3" s="47"/>
-      <c r="C3" s="47"/>
-      <c r="D3" s="47"/>
-      <c r="E3" s="47"/>
-      <c r="F3" s="47"/>
-      <c r="G3" s="47"/>
-      <c r="H3" s="47"/>
-      <c r="I3" s="48"/>
-    </row>
-    <row r="4" spans="1:9" ht="13.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="46"/>
-      <c r="B4" s="47"/>
-      <c r="C4" s="47"/>
-      <c r="D4" s="47"/>
-      <c r="E4" s="47"/>
-      <c r="F4" s="47"/>
-      <c r="G4" s="47"/>
-      <c r="H4" s="47"/>
-      <c r="I4" s="48"/>
-    </row>
-    <row r="5" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="46"/>
-      <c r="B5" s="47"/>
-      <c r="C5" s="47"/>
-      <c r="D5" s="47"/>
-      <c r="E5" s="47"/>
-      <c r="F5" s="47"/>
-      <c r="G5" s="47"/>
-      <c r="H5" s="47"/>
-      <c r="I5" s="48"/>
-    </row>
-    <row r="6" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="49"/>
-      <c r="B6" s="50"/>
-      <c r="C6" s="50"/>
-      <c r="D6" s="50"/>
-      <c r="E6" s="50"/>
-      <c r="F6" s="50"/>
-      <c r="G6" s="50"/>
-      <c r="H6" s="50"/>
-      <c r="I6" s="51"/>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B17" s="17"/>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B18" s="17"/>
-      <c r="D18" s="17"/>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B19" s="17"/>
-      <c r="D19" s="17"/>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B20" s="17"/>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="D21" s="17"/>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B22" s="17"/>
-      <c r="D22" s="17"/>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="D23" s="17"/>
-    </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B24" s="17"/>
-    </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B25" s="17"/>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="58"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="59"/>
+      <c r="B2" s="60"/>
+      <c r="C2" s="60"/>
+      <c r="D2" s="60"/>
+      <c r="E2" s="60"/>
+      <c r="F2" s="60"/>
+      <c r="G2" s="60"/>
+      <c r="H2" s="60"/>
+      <c r="I2" s="61"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="59"/>
+      <c r="B3" s="60"/>
+      <c r="C3" s="60"/>
+      <c r="D3" s="60"/>
+      <c r="E3" s="60"/>
+      <c r="F3" s="60"/>
+      <c r="G3" s="60"/>
+      <c r="H3" s="60"/>
+      <c r="I3" s="61"/>
+    </row>
+    <row r="4" spans="1:9" ht="13" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="59"/>
+      <c r="B4" s="60"/>
+      <c r="C4" s="60"/>
+      <c r="D4" s="60"/>
+      <c r="E4" s="60"/>
+      <c r="F4" s="60"/>
+      <c r="G4" s="60"/>
+      <c r="H4" s="60"/>
+      <c r="I4" s="61"/>
+    </row>
+    <row r="5" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="59"/>
+      <c r="B5" s="60"/>
+      <c r="C5" s="60"/>
+      <c r="D5" s="60"/>
+      <c r="E5" s="60"/>
+      <c r="F5" s="60"/>
+      <c r="G5" s="60"/>
+      <c r="H5" s="60"/>
+      <c r="I5" s="61"/>
+    </row>
+    <row r="6" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="62"/>
+      <c r="B6" s="63"/>
+      <c r="C6" s="63"/>
+      <c r="D6" s="63"/>
+      <c r="E6" s="63"/>
+      <c r="F6" s="63"/>
+      <c r="G6" s="63"/>
+      <c r="H6" s="63"/>
+      <c r="I6" s="64"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>95</v>
+      </c>
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" t="s">
+        <v>72</v>
+      </c>
+      <c r="E9" t="s">
+        <v>73</v>
+      </c>
+      <c r="G9" t="s">
+        <v>86</v>
+      </c>
+      <c r="H9" t="s">
+        <v>73</v>
+      </c>
+      <c r="I9" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="E10" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="G10" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="H10" s="20" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" s="20" t="s">
+        <v>300</v>
+      </c>
+      <c r="B11" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="E11" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="G11" t="s">
+        <v>89</v>
+      </c>
+      <c r="H11" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>96</v>
+      </c>
+      <c r="B12" t="s">
+        <v>43</v>
+      </c>
+      <c r="D12" t="s">
+        <v>81</v>
+      </c>
+      <c r="G12" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="H12" s="20" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>97</v>
+      </c>
+      <c r="B13" t="s">
+        <v>80</v>
+      </c>
+      <c r="D13" t="s">
+        <v>83</v>
+      </c>
+      <c r="G13" t="s">
+        <v>92</v>
+      </c>
+      <c r="H13" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>98</v>
+      </c>
+      <c r="B14" t="s">
+        <v>80</v>
+      </c>
+      <c r="D14" t="s">
+        <v>85</v>
+      </c>
+      <c r="G14" t="s">
+        <v>93</v>
+      </c>
+      <c r="H14" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>99</v>
+      </c>
+      <c r="B15" t="s">
+        <v>43</v>
+      </c>
+      <c r="G15" t="s">
+        <v>94</v>
+      </c>
+      <c r="H15" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>100</v>
+      </c>
+      <c r="B16" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>101</v>
+      </c>
+      <c r="B17" t="s">
+        <v>43</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:I6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="3">
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+  </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A01C55C-4E51-4874-BC12-52D39A06ACCB}">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H48" sqref="H48"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.33203125" customWidth="1"/>
@@ -8294,49 +8451,50 @@
     <col min="8" max="8" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="43" t="s">
+    <row r="1" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="56" t="s">
         <v>293</v>
       </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="45"/>
-    </row>
-    <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="46"/>
-      <c r="B2" s="47"/>
-      <c r="C2" s="47"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
-      <c r="F2" s="48"/>
-    </row>
-    <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="46"/>
-      <c r="B3" s="47"/>
-      <c r="C3" s="47"/>
-      <c r="D3" s="47"/>
-      <c r="E3" s="47"/>
-      <c r="F3" s="48"/>
-    </row>
-    <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="46"/>
-      <c r="B4" s="47"/>
-      <c r="C4" s="47"/>
-      <c r="D4" s="47"/>
-      <c r="E4" s="47"/>
-      <c r="F4" s="48"/>
-    </row>
-    <row r="5" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="49"/>
-      <c r="B5" s="50"/>
-      <c r="C5" s="50"/>
-      <c r="D5" s="50"/>
-      <c r="E5" s="50"/>
-      <c r="F5" s="51"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="58"/>
+    </row>
+    <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="59"/>
+      <c r="B2" s="60"/>
+      <c r="C2" s="60"/>
+      <c r="D2" s="60"/>
+      <c r="E2" s="60"/>
+      <c r="F2" s="61"/>
+    </row>
+    <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="59"/>
+      <c r="B3" s="60"/>
+      <c r="C3" s="60"/>
+      <c r="D3" s="60"/>
+      <c r="E3" s="60"/>
+      <c r="F3" s="61"/>
+    </row>
+    <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="59"/>
+      <c r="B4" s="60"/>
+      <c r="C4" s="60"/>
+      <c r="D4" s="60"/>
+      <c r="E4" s="60"/>
+      <c r="F4" s="61"/>
+      <c r="G4" s="17"/>
+    </row>
+    <row r="5" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="62"/>
+      <c r="B5" s="63"/>
+      <c r="C5" s="63"/>
+      <c r="D5" s="63"/>
+      <c r="E5" s="63"/>
+      <c r="F5" s="64"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>95</v>
       </c>
@@ -8355,8 +8513,11 @@
       <c r="H7" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I7" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="20" t="s">
         <v>23</v>
       </c>
@@ -8376,7 +8537,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="20" t="s">
         <v>300</v>
       </c>
@@ -8396,7 +8557,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>96</v>
       </c>
@@ -8413,7 +8574,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>97</v>
       </c>
@@ -8430,7 +8591,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>98</v>
       </c>
@@ -8447,7 +8608,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>99</v>
       </c>
@@ -8461,7 +8622,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>100</v>
       </c>
@@ -8469,7 +8630,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>101</v>
       </c>
@@ -8498,108 +8659,108 @@
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="43" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" s="56" t="s">
         <v>297</v>
       </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
-      <c r="I1" s="45"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="46"/>
-      <c r="B2" s="47"/>
-      <c r="C2" s="47"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
-      <c r="F2" s="47"/>
-      <c r="G2" s="47"/>
-      <c r="H2" s="47"/>
-      <c r="I2" s="48"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="46"/>
-      <c r="B3" s="47"/>
-      <c r="C3" s="47"/>
-      <c r="D3" s="47"/>
-      <c r="E3" s="47"/>
-      <c r="F3" s="47"/>
-      <c r="G3" s="47"/>
-      <c r="H3" s="47"/>
-      <c r="I3" s="48"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="46"/>
-      <c r="B4" s="47"/>
-      <c r="C4" s="47"/>
-      <c r="D4" s="47"/>
-      <c r="E4" s="47"/>
-      <c r="F4" s="47"/>
-      <c r="G4" s="47"/>
-      <c r="H4" s="47"/>
-      <c r="I4" s="48"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="46"/>
-      <c r="B5" s="47"/>
-      <c r="C5" s="47"/>
-      <c r="D5" s="47"/>
-      <c r="E5" s="47"/>
-      <c r="F5" s="47"/>
-      <c r="G5" s="47"/>
-      <c r="H5" s="47"/>
-      <c r="I5" s="48"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="46"/>
-      <c r="B6" s="47"/>
-      <c r="C6" s="47"/>
-      <c r="D6" s="47"/>
-      <c r="E6" s="47"/>
-      <c r="F6" s="47"/>
-      <c r="G6" s="47"/>
-      <c r="H6" s="47"/>
-      <c r="I6" s="48"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="46"/>
-      <c r="B7" s="47"/>
-      <c r="C7" s="47"/>
-      <c r="D7" s="47"/>
-      <c r="E7" s="47"/>
-      <c r="F7" s="47"/>
-      <c r="G7" s="47"/>
-      <c r="H7" s="47"/>
-      <c r="I7" s="48"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="46"/>
-      <c r="B8" s="47"/>
-      <c r="C8" s="47"/>
-      <c r="D8" s="47"/>
-      <c r="E8" s="47"/>
-      <c r="F8" s="47"/>
-      <c r="G8" s="47"/>
-      <c r="H8" s="47"/>
-      <c r="I8" s="48"/>
-    </row>
-    <row r="9" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="49"/>
-      <c r="B9" s="50"/>
-      <c r="C9" s="50"/>
-      <c r="D9" s="50"/>
-      <c r="E9" s="50"/>
-      <c r="F9" s="50"/>
-      <c r="G9" s="50"/>
-      <c r="H9" s="50"/>
-      <c r="I9" s="51"/>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="58"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="59"/>
+      <c r="B2" s="60"/>
+      <c r="C2" s="60"/>
+      <c r="D2" s="60"/>
+      <c r="E2" s="60"/>
+      <c r="F2" s="60"/>
+      <c r="G2" s="60"/>
+      <c r="H2" s="60"/>
+      <c r="I2" s="61"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="59"/>
+      <c r="B3" s="60"/>
+      <c r="C3" s="60"/>
+      <c r="D3" s="60"/>
+      <c r="E3" s="60"/>
+      <c r="F3" s="60"/>
+      <c r="G3" s="60"/>
+      <c r="H3" s="60"/>
+      <c r="I3" s="61"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="59"/>
+      <c r="B4" s="60"/>
+      <c r="C4" s="60"/>
+      <c r="D4" s="60"/>
+      <c r="E4" s="60"/>
+      <c r="F4" s="60"/>
+      <c r="G4" s="60"/>
+      <c r="H4" s="60"/>
+      <c r="I4" s="61"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="59"/>
+      <c r="B5" s="60"/>
+      <c r="C5" s="60"/>
+      <c r="D5" s="60"/>
+      <c r="E5" s="60"/>
+      <c r="F5" s="60"/>
+      <c r="G5" s="60"/>
+      <c r="H5" s="60"/>
+      <c r="I5" s="61"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="59"/>
+      <c r="B6" s="60"/>
+      <c r="C6" s="60"/>
+      <c r="D6" s="60"/>
+      <c r="E6" s="60"/>
+      <c r="F6" s="60"/>
+      <c r="G6" s="60"/>
+      <c r="H6" s="60"/>
+      <c r="I6" s="61"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="59"/>
+      <c r="B7" s="60"/>
+      <c r="C7" s="60"/>
+      <c r="D7" s="60"/>
+      <c r="E7" s="60"/>
+      <c r="F7" s="60"/>
+      <c r="G7" s="60"/>
+      <c r="H7" s="60"/>
+      <c r="I7" s="61"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="59"/>
+      <c r="B8" s="60"/>
+      <c r="C8" s="60"/>
+      <c r="D8" s="60"/>
+      <c r="E8" s="60"/>
+      <c r="F8" s="60"/>
+      <c r="G8" s="60"/>
+      <c r="H8" s="60"/>
+      <c r="I8" s="61"/>
+    </row>
+    <row r="9" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="62"/>
+      <c r="B9" s="63"/>
+      <c r="C9" s="63"/>
+      <c r="D9" s="63"/>
+      <c r="E9" s="63"/>
+      <c r="F9" s="63"/>
+      <c r="G9" s="63"/>
+      <c r="H9" s="63"/>
+      <c r="I9" s="64"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -8617,56 +8778,56 @@
       <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.109375" customWidth="1"/>
-    <col min="2" max="2" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.1640625" customWidth="1"/>
+    <col min="2" max="2" width="11.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.6640625" customWidth="1"/>
-    <col min="5" max="5" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.44140625" customWidth="1"/>
-    <col min="8" max="8" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.5" customWidth="1"/>
+    <col min="8" max="8" width="11.5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="43" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" s="56" t="s">
         <v>291</v>
       </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="45"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="46"/>
-      <c r="B2" s="47"/>
-      <c r="C2" s="47"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="48"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="46"/>
-      <c r="B3" s="47"/>
-      <c r="C3" s="47"/>
-      <c r="D3" s="47"/>
-      <c r="E3" s="48"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="46"/>
-      <c r="B4" s="47"/>
-      <c r="C4" s="47"/>
-      <c r="D4" s="47"/>
-      <c r="E4" s="48"/>
-    </row>
-    <row r="5" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="49"/>
-      <c r="B5" s="50"/>
-      <c r="C5" s="50"/>
-      <c r="D5" s="50"/>
-      <c r="E5" s="51"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="58"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="59"/>
+      <c r="B2" s="60"/>
+      <c r="C2" s="60"/>
+      <c r="D2" s="60"/>
+      <c r="E2" s="61"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="59"/>
+      <c r="B3" s="60"/>
+      <c r="C3" s="60"/>
+      <c r="D3" s="60"/>
+      <c r="E3" s="61"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="59"/>
+      <c r="B4" s="60"/>
+      <c r="C4" s="60"/>
+      <c r="D4" s="60"/>
+      <c r="E4" s="61"/>
+    </row>
+    <row r="5" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="62"/>
+      <c r="B5" s="63"/>
+      <c r="C5" s="63"/>
+      <c r="D5" s="63"/>
+      <c r="E5" s="64"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>57</v>
       </c>
@@ -8686,7 +8847,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="20" t="s">
         <v>59</v>
       </c>
@@ -8706,7 +8867,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>61</v>
       </c>
@@ -8726,7 +8887,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>63</v>
       </c>
@@ -8746,7 +8907,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>66</v>
       </c>
@@ -8766,7 +8927,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="20" t="s">
         <v>68</v>
       </c>
@@ -8786,7 +8947,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="20" t="s">
         <v>70</v>
       </c>
@@ -8800,7 +8961,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>71</v>
       </c>
@@ -8820,7 +8981,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>74</v>
       </c>
@@ -8840,7 +9001,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>77</v>
       </c>
@@ -8860,7 +9021,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>79</v>
       </c>
@@ -8880,7 +9041,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>82</v>
       </c>
@@ -8900,7 +9061,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="14" t="s">
         <v>84</v>
       </c>
@@ -8920,7 +9081,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>86</v>
       </c>
@@ -8934,7 +9095,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="20" t="s">
         <v>88</v>
       </c>
@@ -8948,7 +9109,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>89</v>
       </c>
@@ -8962,7 +9123,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="20" t="s">
         <v>91</v>
       </c>
@@ -8970,7 +9131,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>92</v>
       </c>
@@ -8978,7 +9139,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>93</v>
       </c>
@@ -8986,7 +9147,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>94</v>
       </c>
@@ -9017,165 +9178,165 @@
       <selection sqref="A1:K11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="43" t="s">
+    <row r="1" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="56" t="s">
         <v>296</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
-      <c r="G1" s="52"/>
-      <c r="H1" s="52"/>
-      <c r="I1" s="52"/>
-      <c r="J1" s="52"/>
-      <c r="K1" s="53"/>
+      <c r="B1" s="65"/>
+      <c r="C1" s="65"/>
+      <c r="D1" s="65"/>
+      <c r="E1" s="65"/>
+      <c r="F1" s="65"/>
+      <c r="G1" s="65"/>
+      <c r="H1" s="65"/>
+      <c r="I1" s="65"/>
+      <c r="J1" s="65"/>
+      <c r="K1" s="66"/>
       <c r="L1" s="19"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" s="54"/>
-      <c r="B2" s="55"/>
-      <c r="C2" s="55"/>
-      <c r="D2" s="55"/>
-      <c r="E2" s="55"/>
-      <c r="F2" s="55"/>
-      <c r="G2" s="55"/>
-      <c r="H2" s="55"/>
-      <c r="I2" s="55"/>
-      <c r="J2" s="55"/>
-      <c r="K2" s="56"/>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2" s="67"/>
+      <c r="B2" s="68"/>
+      <c r="C2" s="68"/>
+      <c r="D2" s="68"/>
+      <c r="E2" s="68"/>
+      <c r="F2" s="68"/>
+      <c r="G2" s="68"/>
+      <c r="H2" s="68"/>
+      <c r="I2" s="68"/>
+      <c r="J2" s="68"/>
+      <c r="K2" s="69"/>
       <c r="L2" s="19"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A3" s="54"/>
-      <c r="B3" s="55"/>
-      <c r="C3" s="55"/>
-      <c r="D3" s="55"/>
-      <c r="E3" s="55"/>
-      <c r="F3" s="55"/>
-      <c r="G3" s="55"/>
-      <c r="H3" s="55"/>
-      <c r="I3" s="55"/>
-      <c r="J3" s="55"/>
-      <c r="K3" s="56"/>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A3" s="67"/>
+      <c r="B3" s="68"/>
+      <c r="C3" s="68"/>
+      <c r="D3" s="68"/>
+      <c r="E3" s="68"/>
+      <c r="F3" s="68"/>
+      <c r="G3" s="68"/>
+      <c r="H3" s="68"/>
+      <c r="I3" s="68"/>
+      <c r="J3" s="68"/>
+      <c r="K3" s="69"/>
       <c r="L3" s="19"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4" s="54"/>
-      <c r="B4" s="55"/>
-      <c r="C4" s="55"/>
-      <c r="D4" s="55"/>
-      <c r="E4" s="55"/>
-      <c r="F4" s="55"/>
-      <c r="G4" s="55"/>
-      <c r="H4" s="55"/>
-      <c r="I4" s="55"/>
-      <c r="J4" s="55"/>
-      <c r="K4" s="56"/>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4" s="67"/>
+      <c r="B4" s="68"/>
+      <c r="C4" s="68"/>
+      <c r="D4" s="68"/>
+      <c r="E4" s="68"/>
+      <c r="F4" s="68"/>
+      <c r="G4" s="68"/>
+      <c r="H4" s="68"/>
+      <c r="I4" s="68"/>
+      <c r="J4" s="68"/>
+      <c r="K4" s="69"/>
       <c r="L4" s="19"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A5" s="54"/>
-      <c r="B5" s="55"/>
-      <c r="C5" s="55"/>
-      <c r="D5" s="55"/>
-      <c r="E5" s="55"/>
-      <c r="F5" s="55"/>
-      <c r="G5" s="55"/>
-      <c r="H5" s="55"/>
-      <c r="I5" s="55"/>
-      <c r="J5" s="55"/>
-      <c r="K5" s="56"/>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A5" s="67"/>
+      <c r="B5" s="68"/>
+      <c r="C5" s="68"/>
+      <c r="D5" s="68"/>
+      <c r="E5" s="68"/>
+      <c r="F5" s="68"/>
+      <c r="G5" s="68"/>
+      <c r="H5" s="68"/>
+      <c r="I5" s="68"/>
+      <c r="J5" s="68"/>
+      <c r="K5" s="69"/>
       <c r="L5" s="19"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6" s="54"/>
-      <c r="B6" s="55"/>
-      <c r="C6" s="55"/>
-      <c r="D6" s="55"/>
-      <c r="E6" s="55"/>
-      <c r="F6" s="55"/>
-      <c r="G6" s="55"/>
-      <c r="H6" s="55"/>
-      <c r="I6" s="55"/>
-      <c r="J6" s="55"/>
-      <c r="K6" s="56"/>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A6" s="67"/>
+      <c r="B6" s="68"/>
+      <c r="C6" s="68"/>
+      <c r="D6" s="68"/>
+      <c r="E6" s="68"/>
+      <c r="F6" s="68"/>
+      <c r="G6" s="68"/>
+      <c r="H6" s="68"/>
+      <c r="I6" s="68"/>
+      <c r="J6" s="68"/>
+      <c r="K6" s="69"/>
       <c r="L6" s="19"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A7" s="54"/>
-      <c r="B7" s="55"/>
-      <c r="C7" s="55"/>
-      <c r="D7" s="55"/>
-      <c r="E7" s="55"/>
-      <c r="F7" s="55"/>
-      <c r="G7" s="55"/>
-      <c r="H7" s="55"/>
-      <c r="I7" s="55"/>
-      <c r="J7" s="55"/>
-      <c r="K7" s="56"/>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A7" s="67"/>
+      <c r="B7" s="68"/>
+      <c r="C7" s="68"/>
+      <c r="D7" s="68"/>
+      <c r="E7" s="68"/>
+      <c r="F7" s="68"/>
+      <c r="G7" s="68"/>
+      <c r="H7" s="68"/>
+      <c r="I7" s="68"/>
+      <c r="J7" s="68"/>
+      <c r="K7" s="69"/>
       <c r="L7" s="19"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A8" s="54"/>
-      <c r="B8" s="55"/>
-      <c r="C8" s="55"/>
-      <c r="D8" s="55"/>
-      <c r="E8" s="55"/>
-      <c r="F8" s="55"/>
-      <c r="G8" s="55"/>
-      <c r="H8" s="55"/>
-      <c r="I8" s="55"/>
-      <c r="J8" s="55"/>
-      <c r="K8" s="56"/>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A8" s="67"/>
+      <c r="B8" s="68"/>
+      <c r="C8" s="68"/>
+      <c r="D8" s="68"/>
+      <c r="E8" s="68"/>
+      <c r="F8" s="68"/>
+      <c r="G8" s="68"/>
+      <c r="H8" s="68"/>
+      <c r="I8" s="68"/>
+      <c r="J8" s="68"/>
+      <c r="K8" s="69"/>
       <c r="L8" s="19"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A9" s="54"/>
-      <c r="B9" s="55"/>
-      <c r="C9" s="55"/>
-      <c r="D9" s="55"/>
-      <c r="E9" s="55"/>
-      <c r="F9" s="55"/>
-      <c r="G9" s="55"/>
-      <c r="H9" s="55"/>
-      <c r="I9" s="55"/>
-      <c r="J9" s="55"/>
-      <c r="K9" s="56"/>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A9" s="67"/>
+      <c r="B9" s="68"/>
+      <c r="C9" s="68"/>
+      <c r="D9" s="68"/>
+      <c r="E9" s="68"/>
+      <c r="F9" s="68"/>
+      <c r="G9" s="68"/>
+      <c r="H9" s="68"/>
+      <c r="I9" s="68"/>
+      <c r="J9" s="68"/>
+      <c r="K9" s="69"/>
       <c r="L9" s="19"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A10" s="54"/>
-      <c r="B10" s="55"/>
-      <c r="C10" s="55"/>
-      <c r="D10" s="55"/>
-      <c r="E10" s="55"/>
-      <c r="F10" s="55"/>
-      <c r="G10" s="55"/>
-      <c r="H10" s="55"/>
-      <c r="I10" s="55"/>
-      <c r="J10" s="55"/>
-      <c r="K10" s="56"/>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A10" s="67"/>
+      <c r="B10" s="68"/>
+      <c r="C10" s="68"/>
+      <c r="D10" s="68"/>
+      <c r="E10" s="68"/>
+      <c r="F10" s="68"/>
+      <c r="G10" s="68"/>
+      <c r="H10" s="68"/>
+      <c r="I10" s="68"/>
+      <c r="J10" s="68"/>
+      <c r="K10" s="69"/>
       <c r="L10" s="19"/>
     </row>
-    <row r="11" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="57"/>
-      <c r="B11" s="58"/>
-      <c r="C11" s="58"/>
-      <c r="D11" s="58"/>
-      <c r="E11" s="58"/>
-      <c r="F11" s="58"/>
-      <c r="G11" s="58"/>
-      <c r="H11" s="58"/>
-      <c r="I11" s="58"/>
-      <c r="J11" s="58"/>
-      <c r="K11" s="59"/>
+    <row r="11" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="70"/>
+      <c r="B11" s="71"/>
+      <c r="C11" s="71"/>
+      <c r="D11" s="71"/>
+      <c r="E11" s="71"/>
+      <c r="F11" s="71"/>
+      <c r="G11" s="71"/>
+      <c r="H11" s="71"/>
+      <c r="I11" s="71"/>
+      <c r="J11" s="71"/>
+      <c r="K11" s="72"/>
       <c r="L11" s="19"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="19"/>
       <c r="B12" s="19"/>
       <c r="C12" s="19"/>
@@ -9189,7 +9350,7 @@
       <c r="K12" s="19"/>
       <c r="L12" s="19"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" s="19"/>
       <c r="B13" s="19"/>
       <c r="C13" s="19"/>
@@ -9203,7 +9364,7 @@
       <c r="K13" s="19"/>
       <c r="L13" s="19"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="19"/>
       <c r="B14" s="19"/>
       <c r="C14" s="19"/>
@@ -9233,27 +9394,27 @@
       <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="41.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.1640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.5" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="19" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="21.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.5" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="20" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="18.44140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>102</v>
       </c>
@@ -9306,7 +9467,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>119</v>
       </c>
@@ -9337,7 +9498,7 @@
       <c r="P2" s="3"/>
       <c r="Q2" s="8"/>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>124</v>
       </c>
@@ -9368,7 +9529,7 @@
       <c r="P3" s="3"/>
       <c r="Q3" s="8"/>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>126</v>
       </c>
@@ -9399,7 +9560,7 @@
       <c r="P4" s="3"/>
       <c r="Q4" s="8"/>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>130</v>
       </c>
@@ -9430,7 +9591,7 @@
       <c r="P5" s="3"/>
       <c r="Q5" s="8"/>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>131</v>
       </c>
@@ -9461,7 +9622,7 @@
       <c r="P6" s="3"/>
       <c r="Q6" s="8"/>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
         <v>134</v>
       </c>
@@ -9492,7 +9653,7 @@
       <c r="P7" s="3"/>
       <c r="Q7" s="8"/>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
         <v>135</v>
       </c>
@@ -9523,7 +9684,7 @@
       <c r="P8" s="3"/>
       <c r="Q8" s="8"/>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
         <v>138</v>
       </c>
@@ -9554,7 +9715,7 @@
       <c r="P9" s="3"/>
       <c r="Q9" s="8"/>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
         <v>139</v>
       </c>
@@ -9585,7 +9746,7 @@
       <c r="P10" s="3"/>
       <c r="Q10" s="8"/>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
         <v>142</v>
       </c>
@@ -9616,7 +9777,7 @@
       <c r="P11" s="3"/>
       <c r="Q11" s="8"/>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
         <v>143</v>
       </c>
@@ -9647,7 +9808,7 @@
       <c r="P12" s="3"/>
       <c r="Q12" s="8"/>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
         <v>146</v>
       </c>
@@ -9678,7 +9839,7 @@
       <c r="P13" s="3"/>
       <c r="Q13" s="8"/>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
         <v>149</v>
       </c>
@@ -9709,7 +9870,7 @@
       <c r="P14" s="3"/>
       <c r="Q14" s="8"/>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
         <v>152</v>
       </c>
@@ -9740,7 +9901,7 @@
       <c r="P15" s="3"/>
       <c r="Q15" s="8"/>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
         <v>155</v>
       </c>
@@ -9771,7 +9932,7 @@
       <c r="P16" s="3"/>
       <c r="Q16" s="8"/>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
         <v>158</v>
       </c>
@@ -9802,7 +9963,7 @@
       <c r="P17" s="3"/>
       <c r="Q17" s="8"/>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
         <v>161</v>
       </c>
@@ -9833,7 +9994,7 @@
       <c r="P18" s="3"/>
       <c r="Q18" s="8"/>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
         <v>164</v>
       </c>
@@ -9864,7 +10025,7 @@
       <c r="P19" s="3"/>
       <c r="Q19" s="8"/>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
         <v>167</v>
       </c>
@@ -9895,7 +10056,7 @@
       <c r="P20" s="3"/>
       <c r="Q20" s="8"/>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="s">
         <v>170</v>
       </c>
@@ -9926,7 +10087,7 @@
       <c r="P21" s="3"/>
       <c r="Q21" s="8"/>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A22" s="6" t="s">
         <v>173</v>
       </c>
@@ -9957,7 +10118,7 @@
       <c r="P22" s="3"/>
       <c r="Q22" s="8"/>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="s">
         <v>176</v>
       </c>
@@ -9988,7 +10149,7 @@
       <c r="P23" s="3"/>
       <c r="Q23" s="8"/>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A24" s="6" t="s">
         <v>179</v>
       </c>
@@ -10019,7 +10180,7 @@
       <c r="P24" s="3"/>
       <c r="Q24" s="8"/>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A25" s="6" t="s">
         <v>182</v>
       </c>
@@ -10050,7 +10211,7 @@
       <c r="P25" s="3"/>
       <c r="Q25" s="8"/>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
         <v>185</v>
       </c>
@@ -10081,7 +10242,7 @@
       <c r="P26" s="3"/>
       <c r="Q26" s="8"/>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A27" s="6" t="s">
         <v>188</v>
       </c>
@@ -10112,7 +10273,7 @@
       <c r="P27" s="3"/>
       <c r="Q27" s="8"/>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A28" s="6" t="s">
         <v>191</v>
       </c>
@@ -10143,7 +10304,7 @@
       <c r="P28" s="3"/>
       <c r="Q28" s="8"/>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A29" s="6" t="s">
         <v>194</v>
       </c>
@@ -10174,7 +10335,7 @@
       <c r="P29" s="3"/>
       <c r="Q29" s="8"/>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A30" s="6" t="s">
         <v>197</v>
       </c>
@@ -10205,7 +10366,7 @@
       <c r="P30" s="3"/>
       <c r="Q30" s="8"/>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A31" s="6" t="s">
         <v>200</v>
       </c>
@@ -10236,7 +10397,7 @@
       <c r="P31" s="3"/>
       <c r="Q31" s="8"/>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A32" s="6" t="s">
         <v>203</v>
       </c>
@@ -10267,7 +10428,7 @@
       <c r="P32" s="3"/>
       <c r="Q32" s="8"/>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A33" s="6" t="s">
         <v>204</v>
       </c>
@@ -10298,7 +10459,7 @@
       <c r="P33" s="3"/>
       <c r="Q33" s="8"/>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A34" s="6" t="s">
         <v>205</v>
       </c>
@@ -10329,7 +10490,7 @@
       <c r="P34" s="3"/>
       <c r="Q34" s="8"/>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A35" s="6" t="s">
         <v>206</v>
       </c>
@@ -10360,7 +10521,7 @@
       <c r="P35" s="3"/>
       <c r="Q35" s="8"/>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A36" s="6" t="s">
         <v>207</v>
       </c>
@@ -10391,7 +10552,7 @@
       <c r="P36" s="3"/>
       <c r="Q36" s="8"/>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A37" s="6" t="s">
         <v>211</v>
       </c>
@@ -10422,7 +10583,7 @@
       <c r="P37" s="3"/>
       <c r="Q37" s="8"/>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A38" s="6" t="s">
         <v>212</v>
       </c>
@@ -10453,7 +10614,7 @@
       <c r="P38" s="3"/>
       <c r="Q38" s="8"/>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A39" s="6" t="s">
         <v>213</v>
       </c>
@@ -10484,7 +10645,7 @@
       <c r="P39" s="3"/>
       <c r="Q39" s="8"/>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A40" s="6" t="s">
         <v>214</v>
       </c>
@@ -10515,7 +10676,7 @@
       <c r="P40" s="3"/>
       <c r="Q40" s="8"/>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A41" s="6" t="s">
         <v>215</v>
       </c>
@@ -10546,7 +10707,7 @@
       <c r="P41" s="3"/>
       <c r="Q41" s="8"/>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A42" s="6" t="s">
         <v>216</v>
       </c>
@@ -10577,7 +10738,7 @@
       <c r="P42" s="3"/>
       <c r="Q42" s="8"/>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A43" s="6" t="s">
         <v>219</v>
       </c>
@@ -10608,7 +10769,7 @@
       <c r="P43" s="3"/>
       <c r="Q43" s="8"/>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A44" s="6" t="s">
         <v>221</v>
       </c>
@@ -10639,7 +10800,7 @@
       <c r="P44" s="3"/>
       <c r="Q44" s="8"/>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A45" s="6" t="s">
         <v>222</v>
       </c>
@@ -10670,7 +10831,7 @@
       <c r="P45" s="3"/>
       <c r="Q45" s="8"/>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A46" s="6" t="s">
         <v>224</v>
       </c>
@@ -10701,7 +10862,7 @@
       <c r="P46" s="3"/>
       <c r="Q46" s="8"/>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A47" s="6" t="s">
         <v>227</v>
       </c>
@@ -10738,7 +10899,7 @@
       <c r="P47" s="3"/>
       <c r="Q47" s="8"/>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A48" s="6" t="s">
         <v>230</v>
       </c>
@@ -10769,7 +10930,7 @@
       <c r="P48" s="3"/>
       <c r="Q48" s="8"/>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A49" s="6" t="s">
         <v>232</v>
       </c>
@@ -10800,7 +10961,7 @@
       <c r="P49" s="3"/>
       <c r="Q49" s="8"/>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A50" s="6" t="s">
         <v>234</v>
       </c>
@@ -10831,7 +10992,7 @@
       <c r="P50" s="3"/>
       <c r="Q50" s="8"/>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A51" s="6" t="s">
         <v>236</v>
       </c>
@@ -10862,7 +11023,7 @@
       <c r="P51" s="3"/>
       <c r="Q51" s="8"/>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A52" s="6" t="s">
         <v>238</v>
       </c>
@@ -10893,7 +11054,7 @@
       <c r="P52" s="3"/>
       <c r="Q52" s="8"/>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A53" s="6" t="s">
         <v>240</v>
       </c>
@@ -10922,7 +11083,7 @@
       <c r="P53" s="3"/>
       <c r="Q53" s="8"/>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A54" s="6" t="s">
         <v>242</v>
       </c>
@@ -10951,7 +11112,7 @@
       <c r="P54" s="3"/>
       <c r="Q54" s="8"/>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A55" s="6" t="s">
         <v>243</v>
       </c>
@@ -10980,7 +11141,7 @@
       <c r="P55" s="3"/>
       <c r="Q55" s="8"/>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A56" s="6" t="s">
         <v>244</v>
       </c>
@@ -11009,7 +11170,7 @@
       <c r="P56" s="3"/>
       <c r="Q56" s="8"/>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A57" s="6" t="s">
         <v>246</v>
       </c>
@@ -11038,7 +11199,7 @@
       <c r="P57" s="3"/>
       <c r="Q57" s="8"/>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A58" s="6" t="s">
         <v>248</v>
       </c>
@@ -11067,7 +11228,7 @@
       <c r="P58" s="3"/>
       <c r="Q58" s="8"/>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A59" s="6" t="s">
         <v>249</v>
       </c>
@@ -11096,7 +11257,7 @@
       <c r="P59" s="3"/>
       <c r="Q59" s="8"/>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A60" s="6" t="s">
         <v>250</v>
       </c>
@@ -11125,7 +11286,7 @@
       <c r="P60" s="3"/>
       <c r="Q60" s="8"/>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A61" s="6" t="s">
         <v>252</v>
       </c>
@@ -11154,7 +11315,7 @@
       <c r="P61" s="3"/>
       <c r="Q61" s="8"/>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A62" s="6" t="s">
         <v>254</v>
       </c>
@@ -11183,7 +11344,7 @@
       <c r="P62" s="3"/>
       <c r="Q62" s="8"/>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A63" s="6" t="s">
         <v>255</v>
       </c>
@@ -11212,7 +11373,7 @@
       <c r="P63" s="3"/>
       <c r="Q63" s="8"/>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A64" s="6" t="s">
         <v>256</v>
       </c>
@@ -11241,7 +11402,7 @@
       <c r="P64" s="3"/>
       <c r="Q64" s="8"/>
     </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A65" s="6" t="s">
         <v>257</v>
       </c>
@@ -11270,7 +11431,7 @@
       <c r="P65" s="3"/>
       <c r="Q65" s="8"/>
     </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A66" s="6" t="s">
         <v>259</v>
       </c>
@@ -11299,7 +11460,7 @@
       <c r="P66" s="3"/>
       <c r="Q66" s="8"/>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A67" s="6" t="s">
         <v>261</v>
       </c>
@@ -11328,7 +11489,7 @@
       <c r="P67" s="3"/>
       <c r="Q67" s="8"/>
     </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A68" s="6" t="s">
         <v>262</v>
       </c>
@@ -11357,7 +11518,7 @@
       <c r="P68" s="3"/>
       <c r="Q68" s="8"/>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A69" s="6" t="s">
         <v>264</v>
       </c>
@@ -11386,7 +11547,7 @@
       <c r="P69" s="3"/>
       <c r="Q69" s="8"/>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A70" s="6" t="s">
         <v>265</v>
       </c>
@@ -11415,7 +11576,7 @@
       <c r="P70" s="3"/>
       <c r="Q70" s="8"/>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A71" s="6" t="s">
         <v>266</v>
       </c>
@@ -11444,7 +11605,7 @@
       <c r="P71" s="3"/>
       <c r="Q71" s="8"/>
     </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A72" s="6" t="s">
         <v>267</v>
       </c>
@@ -11473,7 +11634,7 @@
       <c r="P72" s="3"/>
       <c r="Q72" s="8"/>
     </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A73" s="6" t="s">
         <v>269</v>
       </c>
@@ -11502,7 +11663,7 @@
       <c r="P73" s="3"/>
       <c r="Q73" s="8"/>
     </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A74" s="6" t="s">
         <v>271</v>
       </c>
@@ -11531,7 +11692,7 @@
       <c r="P74" s="3"/>
       <c r="Q74" s="8"/>
     </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A75" s="6" t="s">
         <v>273</v>
       </c>
@@ -11560,7 +11721,7 @@
       <c r="P75" s="3"/>
       <c r="Q75" s="8"/>
     </row>
-    <row r="76" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A76" s="6" t="s">
         <v>274</v>
       </c>
@@ -11589,7 +11750,7 @@
       <c r="P76" s="3"/>
       <c r="Q76" s="8"/>
     </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A77" s="6" t="s">
         <v>275</v>
       </c>
@@ -11618,7 +11779,7 @@
       <c r="P77" s="3"/>
       <c r="Q77" s="8"/>
     </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A78" s="6" t="s">
         <v>276</v>
       </c>
@@ -11647,7 +11808,7 @@
       <c r="P78" s="3"/>
       <c r="Q78" s="8"/>
     </row>
-    <row r="79" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A79" s="6" t="s">
         <v>277</v>
       </c>
@@ -11676,7 +11837,7 @@
       <c r="P79" s="3"/>
       <c r="Q79" s="8"/>
     </row>
-    <row r="80" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A80" s="6" t="s">
         <v>279</v>
       </c>
@@ -11705,7 +11866,7 @@
       <c r="P80" s="3"/>
       <c r="Q80" s="8"/>
     </row>
-    <row r="81" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A81" s="6" t="s">
         <v>281</v>
       </c>
@@ -11734,7 +11895,7 @@
       <c r="P81" s="3"/>
       <c r="Q81" s="8"/>
     </row>
-    <row r="82" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A82" s="6" t="s">
         <v>282</v>
       </c>
@@ -11763,7 +11924,7 @@
       <c r="P82" s="3"/>
       <c r="Q82" s="8"/>
     </row>
-    <row r="83" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A83" s="6" t="s">
         <v>283</v>
       </c>
@@ -11792,7 +11953,7 @@
       <c r="P83" s="3"/>
       <c r="Q83" s="8"/>
     </row>
-    <row r="84" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A84" s="6" t="s">
         <v>285</v>
       </c>
@@ -11819,7 +11980,7 @@
       <c r="P84" s="3"/>
       <c r="Q84" s="8"/>
     </row>
-    <row r="85" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A85" s="6" t="s">
         <v>288</v>
       </c>
@@ -11846,7 +12007,7 @@
       <c r="P85" s="3"/>
       <c r="Q85" s="8"/>
     </row>
-    <row r="86" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A86" s="6" t="s">
         <v>289</v>
       </c>

</xml_diff>

<commit_message>
Update POS - Database Tracker.xlsx
</commit_message>
<xml_diff>
--- a/docs/Database Tables Outlines/POS - Database Tracker.xlsx
+++ b/docs/Database Tables Outlines/POS - Database Tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/XAMPP/xamppfiles/htdocs/CPS353-POS/docs/Database Tables Outlines/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4D38EAE-C40E-E241-AA0E-1CED06F55934}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76F73DDC-07B7-894B-BFF5-B8BC41FCBE63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14100" firstSheet="6" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DOCS" sheetId="3" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1472" uniqueCount="476">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1486" uniqueCount="481">
   <si>
     <t xml:space="preserve">table name </t>
   </si>
@@ -1728,6 +1728,21 @@
   </si>
   <si>
     <t>Birdie</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>first_name</t>
+  </si>
+  <si>
+    <t>last_name</t>
+  </si>
+  <si>
+    <t>address</t>
+  </si>
+  <si>
+    <t>customers</t>
   </si>
 </sst>
 </file>
@@ -2232,7 +2247,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -2319,6 +2334,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -2370,34 +2386,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="70">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
@@ -2966,6 +2963,28 @@
         <horizontal style="thin">
           <color indexed="64"/>
         </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -3974,47 +3993,47 @@
     <tableColumn id="3" xr3:uid="{9F069C76-EAD1-3948-8AE5-0CF6C28955AB}" name="prod_description" dataDxfId="33"/>
     <tableColumn id="4" xr3:uid="{2E613335-9BE1-0948-A582-1540033DE6C8}" name="prod_image" dataDxfId="32"/>
     <tableColumn id="13" xr3:uid="{1104D79E-9A5A-714B-AF17-C62ED3207498}" name="Vendor Name (temp until we have the vendor ID Populated)" dataDxfId="31"/>
-    <tableColumn id="15" xr3:uid="{096071DB-C10F-F440-8999-1F42847DAA46}" name="prod_quantity" dataDxfId="0"/>
-    <tableColumn id="5" xr3:uid="{D5D64163-4784-BD4D-AAE1-2E1E9CE75F46}" name="VENDOR_ID" dataDxfId="30"/>
-    <tableColumn id="14" xr3:uid="{2A3F3825-722E-7C46-9D1A-5C1230676C9D}" name="Prod Category (temp until we have Category ID" dataDxfId="29"/>
-    <tableColumn id="6" xr3:uid="{25872DA6-C700-8343-9B2D-5AC26C6CF8F8}" name="PRODUCT_CATEGORY" dataDxfId="28"/>
-    <tableColumn id="7" xr3:uid="{568DF9DC-F623-E243-86FB-5FB51D02A417}" name="pr_brand" dataDxfId="27"/>
-    <tableColumn id="8" xr3:uid="{F86E5636-7B76-F84C-A4F4-AA76B3DD7EAA}" name="pr_model" dataDxfId="26"/>
-    <tableColumn id="9" xr3:uid="{535CC5DA-5633-1D4B-913C-584159C934AD}" name="prod_date_purchased" dataDxfId="25"/>
-    <tableColumn id="10" xr3:uid="{7F3480CA-2C56-CF4C-8CD8-6424C21705DA}" name="prod_purchase_cost" dataDxfId="24"/>
-    <tableColumn id="11" xr3:uid="{1502990D-7EF5-224C-B7E0-96F3D3F1B0E1}" name="prod_rental_cost" dataDxfId="23"/>
-    <tableColumn id="12" xr3:uid="{6CAF6211-E949-3547-9185-BEF0E1373142}" name="prod_retail_cost" dataDxfId="22"/>
+    <tableColumn id="15" xr3:uid="{096071DB-C10F-F440-8999-1F42847DAA46}" name="prod_quantity" dataDxfId="30"/>
+    <tableColumn id="5" xr3:uid="{D5D64163-4784-BD4D-AAE1-2E1E9CE75F46}" name="VENDOR_ID" dataDxfId="29"/>
+    <tableColumn id="14" xr3:uid="{2A3F3825-722E-7C46-9D1A-5C1230676C9D}" name="Prod Category (temp until we have Category ID" dataDxfId="28"/>
+    <tableColumn id="6" xr3:uid="{25872DA6-C700-8343-9B2D-5AC26C6CF8F8}" name="PRODUCT_CATEGORY" dataDxfId="27"/>
+    <tableColumn id="7" xr3:uid="{568DF9DC-F623-E243-86FB-5FB51D02A417}" name="pr_brand" dataDxfId="26"/>
+    <tableColumn id="8" xr3:uid="{F86E5636-7B76-F84C-A4F4-AA76B3DD7EAA}" name="pr_model" dataDxfId="25"/>
+    <tableColumn id="9" xr3:uid="{535CC5DA-5633-1D4B-913C-584159C934AD}" name="prod_date_purchased" dataDxfId="24"/>
+    <tableColumn id="10" xr3:uid="{7F3480CA-2C56-CF4C-8CD8-6424C21705DA}" name="prod_purchase_cost" dataDxfId="23"/>
+    <tableColumn id="11" xr3:uid="{1502990D-7EF5-224C-B7E0-96F3D3F1B0E1}" name="prod_rental_cost" dataDxfId="22"/>
+    <tableColumn id="12" xr3:uid="{6CAF6211-E949-3547-9185-BEF0E1373142}" name="prod_retail_cost" dataDxfId="21"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table24.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="23" xr:uid="{B41F1D88-6BC9-7541-8EAA-179233B1D5E9}" name="Table23" displayName="Table23" ref="A1:E4" totalsRowShown="0" headerRowDxfId="21" headerRowBorderDxfId="20" tableBorderDxfId="19" totalsRowBorderDxfId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="23" xr:uid="{B41F1D88-6BC9-7541-8EAA-179233B1D5E9}" name="Table23" displayName="Table23" ref="A1:E4" totalsRowShown="0" headerRowDxfId="20" headerRowBorderDxfId="19" tableBorderDxfId="18" totalsRowBorderDxfId="17">
   <autoFilter ref="A1:E4" xr:uid="{B41F1D88-6BC9-7541-8EAA-179233B1D5E9}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{D4BE343A-ABA6-EA42-A6F4-73F5923DD7E1}" name="MEMBERSHIP_ID" dataDxfId="17"/>
-    <tableColumn id="2" xr3:uid="{AF8BB9C8-1D59-3244-8953-60FEDD92B512}" name="USER_ID" dataDxfId="16"/>
-    <tableColumn id="3" xr3:uid="{2F1F6E59-B988-BC43-BCF0-9ACE635AD7F3}" name="mem_type" dataDxfId="15"/>
-    <tableColumn id="4" xr3:uid="{E4E63878-CBB6-854E-A200-804EB41A984C}" name="mem_cost" dataDxfId="14"/>
-    <tableColumn id="5" xr3:uid="{CDCE100B-6B9F-4B4F-8B08-F44E7A548EC6}" name="mem_duration" dataDxfId="13"/>
+    <tableColumn id="1" xr3:uid="{D4BE343A-ABA6-EA42-A6F4-73F5923DD7E1}" name="MEMBERSHIP_ID" dataDxfId="16"/>
+    <tableColumn id="2" xr3:uid="{AF8BB9C8-1D59-3244-8953-60FEDD92B512}" name="USER_ID" dataDxfId="15"/>
+    <tableColumn id="3" xr3:uid="{2F1F6E59-B988-BC43-BCF0-9ACE635AD7F3}" name="mem_type" dataDxfId="14"/>
+    <tableColumn id="4" xr3:uid="{E4E63878-CBB6-854E-A200-804EB41A984C}" name="mem_cost" dataDxfId="13"/>
+    <tableColumn id="5" xr3:uid="{CDCE100B-6B9F-4B4F-8B08-F44E7A548EC6}" name="mem_duration" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table25.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="24" xr:uid="{E333897C-4734-8E49-9F1A-8F1B50120560}" name="Table24" displayName="Table24" ref="A7:H14" totalsRowShown="0" headerRowDxfId="12" headerRowBorderDxfId="11" tableBorderDxfId="10" totalsRowBorderDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="24" xr:uid="{E333897C-4734-8E49-9F1A-8F1B50120560}" name="Table24" displayName="Table24" ref="A7:H14" totalsRowShown="0" headerRowDxfId="11" headerRowBorderDxfId="10" tableBorderDxfId="9" totalsRowBorderDxfId="8">
   <autoFilter ref="A7:H14" xr:uid="{E333897C-4734-8E49-9F1A-8F1B50120560}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{206B337B-A861-B940-B7D9-E9FB76B9F6BD}" name="CLASS_ID" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{F8B76A29-B663-D94A-9110-027E02E2498D}" name="class_name" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{9A937EA6-E1CB-4941-BBAA-AD7C05972803}" name="EMPLOYEE_ID" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{52F747A5-59A0-D14E-A225-F7D289115DC7}" name="class_description" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{014BD5EC-4461-6A45-B6D4-36D61480B55E}" name="class_image" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{DA5B623B-8894-0649-B5B7-3A92B570CB76}" name="class_max_capacity" dataDxfId="3"/>
-    <tableColumn id="7" xr3:uid="{85BAB98E-E9E2-DE4A-ADAD-5038312C5D4E}" name="class_time" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{0155195F-AA32-8941-8A1D-EE52717632FA}" name="class_day" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{206B337B-A861-B940-B7D9-E9FB76B9F6BD}" name="CLASS_ID" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{F8B76A29-B663-D94A-9110-027E02E2498D}" name="class_name" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{9A937EA6-E1CB-4941-BBAA-AD7C05972803}" name="EMPLOYEE_ID" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{52F747A5-59A0-D14E-A225-F7D289115DC7}" name="class_description" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{014BD5EC-4461-6A45-B6D4-36D61480B55E}" name="class_image" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{DA5B623B-8894-0649-B5B7-3A92B570CB76}" name="class_max_capacity" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{85BAB98E-E9E2-DE4A-ADAD-5038312C5D4E}" name="class_time" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{0155195F-AA32-8941-8A1D-EE52717632FA}" name="class_day" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4483,7 +4502,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40455DF4-3F31-4947-BCA7-1853A71C76DD}">
   <dimension ref="A1:O131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A105" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="A105" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="F128" sqref="F128"/>
     </sheetView>
   </sheetViews>
@@ -4564,7 +4583,7 @@
       <c r="E2" s="35" t="s">
         <v>116</v>
       </c>
-      <c r="F2" s="79"/>
+      <c r="F2" s="62"/>
       <c r="G2" s="26"/>
       <c r="H2" s="36" t="s">
         <v>299</v>
@@ -4591,7 +4610,7 @@
       <c r="E3" s="35" t="s">
         <v>116</v>
       </c>
-      <c r="F3" s="79"/>
+      <c r="F3" s="62"/>
       <c r="G3" s="29"/>
       <c r="H3" s="36" t="s">
         <v>299</v>
@@ -4618,7 +4637,7 @@
       <c r="E4" s="35" t="s">
         <v>116</v>
       </c>
-      <c r="F4" s="79"/>
+      <c r="F4" s="62"/>
       <c r="G4" s="29"/>
       <c r="H4" s="36" t="s">
         <v>299</v>
@@ -4645,7 +4664,7 @@
       <c r="E5" s="35" t="s">
         <v>116</v>
       </c>
-      <c r="F5" s="79"/>
+      <c r="F5" s="62"/>
       <c r="G5" s="29"/>
       <c r="H5" s="36" t="s">
         <v>299</v>
@@ -4672,7 +4691,7 @@
       <c r="E6" s="35" t="s">
         <v>116</v>
       </c>
-      <c r="F6" s="79"/>
+      <c r="F6" s="62"/>
       <c r="G6" s="29"/>
       <c r="H6" s="36" t="s">
         <v>299</v>
@@ -4699,7 +4718,7 @@
       <c r="E7" s="35" t="s">
         <v>116</v>
       </c>
-      <c r="F7" s="79"/>
+      <c r="F7" s="62"/>
       <c r="G7" s="29"/>
       <c r="H7" s="36" t="s">
         <v>299</v>
@@ -4726,7 +4745,7 @@
       <c r="E8" s="35" t="s">
         <v>116</v>
       </c>
-      <c r="F8" s="79"/>
+      <c r="F8" s="62"/>
       <c r="G8" s="29"/>
       <c r="H8" s="36" t="s">
         <v>299</v>
@@ -4753,7 +4772,7 @@
       <c r="E9" s="35" t="s">
         <v>116</v>
       </c>
-      <c r="F9" s="79"/>
+      <c r="F9" s="62"/>
       <c r="G9" s="29"/>
       <c r="H9" s="36" t="s">
         <v>299</v>
@@ -4780,7 +4799,7 @@
       <c r="E10" s="35" t="s">
         <v>116</v>
       </c>
-      <c r="F10" s="79"/>
+      <c r="F10" s="62"/>
       <c r="G10" s="29"/>
       <c r="H10" s="36" t="s">
         <v>299</v>
@@ -4807,7 +4826,7 @@
       <c r="E11" s="35" t="s">
         <v>116</v>
       </c>
-      <c r="F11" s="79"/>
+      <c r="F11" s="62"/>
       <c r="G11" s="29"/>
       <c r="H11" s="36" t="s">
         <v>299</v>
@@ -4834,7 +4853,7 @@
       <c r="E12" s="35" t="s">
         <v>116</v>
       </c>
-      <c r="F12" s="79"/>
+      <c r="F12" s="62"/>
       <c r="G12" s="29"/>
       <c r="H12" s="36" t="s">
         <v>299</v>
@@ -4861,7 +4880,7 @@
       <c r="E13" s="35" t="s">
         <v>116</v>
       </c>
-      <c r="F13" s="79"/>
+      <c r="F13" s="62"/>
       <c r="G13" s="29"/>
       <c r="H13" s="36" t="s">
         <v>299</v>
@@ -4888,7 +4907,7 @@
       <c r="E14" s="35" t="s">
         <v>116</v>
       </c>
-      <c r="F14" s="79"/>
+      <c r="F14" s="62"/>
       <c r="G14" s="29"/>
       <c r="H14" s="36" t="s">
         <v>299</v>
@@ -4915,7 +4934,7 @@
       <c r="E15" s="35" t="s">
         <v>116</v>
       </c>
-      <c r="F15" s="79"/>
+      <c r="F15" s="62"/>
       <c r="G15" s="29"/>
       <c r="H15" s="36" t="s">
         <v>299</v>
@@ -4942,7 +4961,7 @@
       <c r="E16" s="35" t="s">
         <v>116</v>
       </c>
-      <c r="F16" s="79"/>
+      <c r="F16" s="62"/>
       <c r="G16" s="29"/>
       <c r="H16" s="36" t="s">
         <v>299</v>
@@ -4969,7 +4988,7 @@
       <c r="E17" s="35" t="s">
         <v>116</v>
       </c>
-      <c r="F17" s="79"/>
+      <c r="F17" s="62"/>
       <c r="G17" s="29"/>
       <c r="H17" s="36" t="s">
         <v>299</v>
@@ -4996,7 +5015,7 @@
       <c r="E18" s="35" t="s">
         <v>116</v>
       </c>
-      <c r="F18" s="79"/>
+      <c r="F18" s="62"/>
       <c r="G18" s="29"/>
       <c r="H18" s="36" t="s">
         <v>299</v>
@@ -5023,7 +5042,7 @@
       <c r="E19" s="35" t="s">
         <v>116</v>
       </c>
-      <c r="F19" s="79"/>
+      <c r="F19" s="62"/>
       <c r="G19" s="29"/>
       <c r="H19" s="36" t="s">
         <v>299</v>
@@ -5050,7 +5069,7 @@
       <c r="E20" s="35" t="s">
         <v>116</v>
       </c>
-      <c r="F20" s="79"/>
+      <c r="F20" s="62"/>
       <c r="G20" s="29"/>
       <c r="H20" s="36" t="s">
         <v>299</v>
@@ -5077,7 +5096,7 @@
       <c r="E21" s="35" t="s">
         <v>236</v>
       </c>
-      <c r="F21" s="79"/>
+      <c r="F21" s="62"/>
       <c r="G21" s="29"/>
       <c r="H21" s="36" t="s">
         <v>299</v>
@@ -5104,7 +5123,7 @@
       <c r="E22" s="35" t="s">
         <v>236</v>
       </c>
-      <c r="F22" s="79"/>
+      <c r="F22" s="62"/>
       <c r="G22" s="29"/>
       <c r="H22" s="36" t="s">
         <v>299</v>
@@ -5131,7 +5150,7 @@
       <c r="E23" s="35" t="s">
         <v>236</v>
       </c>
-      <c r="F23" s="79"/>
+      <c r="F23" s="62"/>
       <c r="G23" s="29"/>
       <c r="H23" s="36" t="s">
         <v>299</v>
@@ -5158,7 +5177,7 @@
       <c r="E24" s="35" t="s">
         <v>236</v>
       </c>
-      <c r="F24" s="79"/>
+      <c r="F24" s="62"/>
       <c r="G24" s="29"/>
       <c r="H24" s="36" t="s">
         <v>299</v>
@@ -5185,7 +5204,7 @@
       <c r="E25" s="35" t="s">
         <v>236</v>
       </c>
-      <c r="F25" s="79"/>
+      <c r="F25" s="62"/>
       <c r="G25" s="29"/>
       <c r="H25" s="36" t="s">
         <v>299</v>
@@ -5212,7 +5231,7 @@
       <c r="E26" s="35" t="s">
         <v>236</v>
       </c>
-      <c r="F26" s="79"/>
+      <c r="F26" s="62"/>
       <c r="G26" s="29"/>
       <c r="H26" s="36" t="s">
         <v>299</v>
@@ -5239,7 +5258,7 @@
       <c r="E27" s="35" t="s">
         <v>236</v>
       </c>
-      <c r="F27" s="79"/>
+      <c r="F27" s="62"/>
       <c r="G27" s="29"/>
       <c r="H27" s="36" t="s">
         <v>299</v>
@@ -5266,7 +5285,7 @@
       <c r="E28" s="35" t="s">
         <v>236</v>
       </c>
-      <c r="F28" s="79"/>
+      <c r="F28" s="62"/>
       <c r="G28" s="29"/>
       <c r="H28" s="36" t="s">
         <v>299</v>
@@ -5293,7 +5312,7 @@
       <c r="E29" s="35" t="s">
         <v>236</v>
       </c>
-      <c r="F29" s="79"/>
+      <c r="F29" s="62"/>
       <c r="G29" s="29"/>
       <c r="H29" s="36" t="s">
         <v>299</v>
@@ -5320,7 +5339,7 @@
       <c r="E30" s="35" t="s">
         <v>236</v>
       </c>
-      <c r="F30" s="79"/>
+      <c r="F30" s="62"/>
       <c r="G30" s="29"/>
       <c r="H30" s="36" t="s">
         <v>299</v>
@@ -5347,7 +5366,7 @@
       <c r="E31" s="35" t="s">
         <v>236</v>
       </c>
-      <c r="F31" s="79"/>
+      <c r="F31" s="62"/>
       <c r="G31" s="29"/>
       <c r="H31" s="36" t="s">
         <v>299</v>
@@ -5374,7 +5393,7 @@
       <c r="E32" s="35" t="s">
         <v>236</v>
       </c>
-      <c r="F32" s="79"/>
+      <c r="F32" s="62"/>
       <c r="G32" s="29"/>
       <c r="H32" s="36" t="s">
         <v>299</v>
@@ -5401,7 +5420,7 @@
       <c r="E33" s="35" t="s">
         <v>236</v>
       </c>
-      <c r="F33" s="79"/>
+      <c r="F33" s="62"/>
       <c r="G33" s="29"/>
       <c r="H33" s="36" t="s">
         <v>299</v>
@@ -5428,7 +5447,7 @@
       <c r="E34" s="35" t="s">
         <v>236</v>
       </c>
-      <c r="F34" s="79"/>
+      <c r="F34" s="62"/>
       <c r="G34" s="29"/>
       <c r="H34" s="36" t="s">
         <v>299</v>
@@ -5455,7 +5474,7 @@
       <c r="E35" s="35" t="s">
         <v>236</v>
       </c>
-      <c r="F35" s="79"/>
+      <c r="F35" s="62"/>
       <c r="G35" s="29"/>
       <c r="H35" s="36" t="s">
         <v>299</v>
@@ -5482,7 +5501,7 @@
       <c r="E36" s="35" t="s">
         <v>236</v>
       </c>
-      <c r="F36" s="79"/>
+      <c r="F36" s="62"/>
       <c r="G36" s="29"/>
       <c r="H36" s="36" t="s">
         <v>299</v>
@@ -5509,7 +5528,7 @@
       <c r="E37" s="35" t="s">
         <v>236</v>
       </c>
-      <c r="F37" s="79"/>
+      <c r="F37" s="62"/>
       <c r="G37" s="29"/>
       <c r="H37" s="36" t="s">
         <v>299</v>
@@ -5536,7 +5555,7 @@
       <c r="E38" s="35" t="s">
         <v>236</v>
       </c>
-      <c r="F38" s="79"/>
+      <c r="F38" s="62"/>
       <c r="G38" s="29"/>
       <c r="H38" s="36" t="s">
         <v>299</v>
@@ -5563,7 +5582,7 @@
       <c r="E39" s="35" t="s">
         <v>236</v>
       </c>
-      <c r="F39" s="79"/>
+      <c r="F39" s="62"/>
       <c r="G39" s="29"/>
       <c r="H39" s="36" t="s">
         <v>299</v>
@@ -5590,7 +5609,7 @@
       <c r="E40" s="35" t="s">
         <v>236</v>
       </c>
-      <c r="F40" s="79"/>
+      <c r="F40" s="62"/>
       <c r="G40" s="29"/>
       <c r="H40" s="36" t="s">
         <v>299</v>
@@ -5617,7 +5636,7 @@
       <c r="E41" s="35" t="s">
         <v>236</v>
       </c>
-      <c r="F41" s="79"/>
+      <c r="F41" s="62"/>
       <c r="G41" s="29"/>
       <c r="H41" s="36" t="s">
         <v>299</v>
@@ -5644,7 +5663,7 @@
       <c r="E42" s="35" t="s">
         <v>236</v>
       </c>
-      <c r="F42" s="79"/>
+      <c r="F42" s="62"/>
       <c r="G42" s="29"/>
       <c r="H42" s="36" t="s">
         <v>299</v>
@@ -5671,7 +5690,7 @@
       <c r="E43" s="35" t="s">
         <v>236</v>
       </c>
-      <c r="F43" s="79"/>
+      <c r="F43" s="62"/>
       <c r="G43" s="29"/>
       <c r="H43" s="36" t="s">
         <v>299</v>
@@ -5698,7 +5717,7 @@
       <c r="E44" s="35" t="s">
         <v>123</v>
       </c>
-      <c r="F44" s="79"/>
+      <c r="F44" s="62"/>
       <c r="G44" s="29"/>
       <c r="H44" s="36" t="s">
         <v>299</v>
@@ -5725,7 +5744,7 @@
       <c r="E45" s="35" t="s">
         <v>123</v>
       </c>
-      <c r="F45" s="79"/>
+      <c r="F45" s="62"/>
       <c r="G45" s="29"/>
       <c r="H45" s="36" t="s">
         <v>299</v>
@@ -5752,7 +5771,7 @@
       <c r="E46" s="35" t="s">
         <v>123</v>
       </c>
-      <c r="F46" s="79"/>
+      <c r="F46" s="62"/>
       <c r="G46" s="29"/>
       <c r="H46" s="36" t="s">
         <v>299</v>
@@ -5779,7 +5798,7 @@
       <c r="E47" s="35" t="s">
         <v>123</v>
       </c>
-      <c r="F47" s="79"/>
+      <c r="F47" s="62"/>
       <c r="G47" s="29"/>
       <c r="H47" s="36" t="s">
         <v>299</v>
@@ -5806,7 +5825,7 @@
       <c r="E48" s="35" t="s">
         <v>123</v>
       </c>
-      <c r="F48" s="79"/>
+      <c r="F48" s="62"/>
       <c r="G48" s="29"/>
       <c r="H48" s="36" t="s">
         <v>299</v>
@@ -5833,7 +5852,7 @@
       <c r="E49" s="35" t="s">
         <v>123</v>
       </c>
-      <c r="F49" s="79"/>
+      <c r="F49" s="62"/>
       <c r="G49" s="29"/>
       <c r="H49" s="36" t="s">
         <v>299</v>
@@ -5860,7 +5879,7 @@
       <c r="E50" s="35" t="s">
         <v>123</v>
       </c>
-      <c r="F50" s="79"/>
+      <c r="F50" s="62"/>
       <c r="G50" s="29"/>
       <c r="H50" s="36" t="s">
         <v>299</v>
@@ -5887,7 +5906,7 @@
       <c r="E51" s="35" t="s">
         <v>123</v>
       </c>
-      <c r="F51" s="79"/>
+      <c r="F51" s="62"/>
       <c r="G51" s="29"/>
       <c r="H51" s="36" t="s">
         <v>299</v>
@@ -5914,7 +5933,7 @@
       <c r="E52" s="35" t="s">
         <v>123</v>
       </c>
-      <c r="F52" s="79"/>
+      <c r="F52" s="62"/>
       <c r="G52" s="29"/>
       <c r="H52" s="36" t="s">
         <v>299</v>
@@ -5941,7 +5960,7 @@
       <c r="E53" s="35" t="s">
         <v>123</v>
       </c>
-      <c r="F53" s="79"/>
+      <c r="F53" s="62"/>
       <c r="G53" s="29"/>
       <c r="H53" s="36" t="s">
         <v>299</v>
@@ -5968,7 +5987,7 @@
       <c r="E54" s="35" t="s">
         <v>123</v>
       </c>
-      <c r="F54" s="79"/>
+      <c r="F54" s="62"/>
       <c r="G54" s="29"/>
       <c r="H54" s="36" t="s">
         <v>299</v>
@@ -5995,7 +6014,7 @@
       <c r="E55" s="35" t="s">
         <v>123</v>
       </c>
-      <c r="F55" s="79"/>
+      <c r="F55" s="62"/>
       <c r="G55" s="29"/>
       <c r="H55" s="36" t="s">
         <v>299</v>
@@ -6022,7 +6041,7 @@
       <c r="E56" s="35" t="s">
         <v>123</v>
       </c>
-      <c r="F56" s="79"/>
+      <c r="F56" s="62"/>
       <c r="G56" s="29"/>
       <c r="H56" s="36" t="s">
         <v>299</v>
@@ -6049,7 +6068,7 @@
       <c r="E57" s="35" t="s">
         <v>123</v>
       </c>
-      <c r="F57" s="79"/>
+      <c r="F57" s="62"/>
       <c r="G57" s="29"/>
       <c r="H57" s="36" t="s">
         <v>299</v>
@@ -6076,7 +6095,7 @@
       <c r="E58" s="35" t="s">
         <v>123</v>
       </c>
-      <c r="F58" s="79"/>
+      <c r="F58" s="62"/>
       <c r="G58" s="29"/>
       <c r="H58" s="36" t="s">
         <v>299</v>
@@ -6103,7 +6122,7 @@
       <c r="E59" s="35" t="s">
         <v>123</v>
       </c>
-      <c r="F59" s="79"/>
+      <c r="F59" s="62"/>
       <c r="G59" s="29"/>
       <c r="H59" s="36" t="s">
         <v>299</v>
@@ -6130,7 +6149,7 @@
       <c r="E60" s="35" t="s">
         <v>123</v>
       </c>
-      <c r="F60" s="79"/>
+      <c r="F60" s="62"/>
       <c r="G60" s="29"/>
       <c r="H60" s="36" t="s">
         <v>299</v>
@@ -6157,7 +6176,7 @@
       <c r="E61" s="35" t="s">
         <v>123</v>
       </c>
-      <c r="F61" s="79"/>
+      <c r="F61" s="62"/>
       <c r="G61" s="29"/>
       <c r="H61" s="36" t="s">
         <v>299</v>
@@ -6184,7 +6203,7 @@
       <c r="E62" s="35" t="s">
         <v>123</v>
       </c>
-      <c r="F62" s="79"/>
+      <c r="F62" s="62"/>
       <c r="G62" s="29"/>
       <c r="H62" s="36" t="s">
         <v>299</v>
@@ -6211,7 +6230,7 @@
       <c r="E63" s="35" t="s">
         <v>123</v>
       </c>
-      <c r="F63" s="79"/>
+      <c r="F63" s="62"/>
       <c r="G63" s="29"/>
       <c r="H63" s="36" t="s">
         <v>299</v>
@@ -6238,7 +6257,7 @@
       <c r="E64" s="35" t="s">
         <v>123</v>
       </c>
-      <c r="F64" s="79"/>
+      <c r="F64" s="62"/>
       <c r="G64" s="29"/>
       <c r="H64" s="36" t="s">
         <v>299</v>
@@ -6265,7 +6284,7 @@
       <c r="E65" s="35" t="s">
         <v>123</v>
       </c>
-      <c r="F65" s="79"/>
+      <c r="F65" s="62"/>
       <c r="G65" s="29"/>
       <c r="H65" s="36" t="s">
         <v>299</v>
@@ -6292,7 +6311,7 @@
       <c r="E66" s="35" t="s">
         <v>123</v>
       </c>
-      <c r="F66" s="79"/>
+      <c r="F66" s="62"/>
       <c r="G66" s="29"/>
       <c r="H66" s="36" t="s">
         <v>299</v>
@@ -6319,7 +6338,7 @@
       <c r="E67" s="35" t="s">
         <v>123</v>
       </c>
-      <c r="F67" s="79"/>
+      <c r="F67" s="62"/>
       <c r="G67" s="29"/>
       <c r="H67" s="36" t="s">
         <v>299</v>
@@ -6346,7 +6365,7 @@
       <c r="E68" s="35" t="s">
         <v>123</v>
       </c>
-      <c r="F68" s="79"/>
+      <c r="F68" s="62"/>
       <c r="G68" s="29"/>
       <c r="H68" s="36" t="s">
         <v>299</v>
@@ -6373,7 +6392,7 @@
       <c r="E69" s="35" t="s">
         <v>123</v>
       </c>
-      <c r="F69" s="79"/>
+      <c r="F69" s="62"/>
       <c r="G69" s="29"/>
       <c r="H69" s="36" t="s">
         <v>299</v>
@@ -6400,7 +6419,7 @@
       <c r="E70" s="35" t="s">
         <v>123</v>
       </c>
-      <c r="F70" s="79"/>
+      <c r="F70" s="62"/>
       <c r="G70" s="29"/>
       <c r="H70" s="36" t="s">
         <v>299</v>
@@ -6427,7 +6446,7 @@
       <c r="E71" s="35" t="s">
         <v>123</v>
       </c>
-      <c r="F71" s="79"/>
+      <c r="F71" s="62"/>
       <c r="G71" s="29"/>
       <c r="H71" s="36" t="s">
         <v>299</v>
@@ -6454,7 +6473,7 @@
       <c r="E72" s="35" t="s">
         <v>123</v>
       </c>
-      <c r="F72" s="79"/>
+      <c r="F72" s="62"/>
       <c r="G72" s="29"/>
       <c r="H72" s="36" t="s">
         <v>299</v>
@@ -6481,7 +6500,7 @@
       <c r="E73" s="35" t="s">
         <v>123</v>
       </c>
-      <c r="F73" s="79"/>
+      <c r="F73" s="62"/>
       <c r="G73" s="29"/>
       <c r="H73" s="36" t="s">
         <v>299</v>
@@ -6508,7 +6527,7 @@
       <c r="E74" s="35" t="s">
         <v>123</v>
       </c>
-      <c r="F74" s="79"/>
+      <c r="F74" s="62"/>
       <c r="G74" s="29"/>
       <c r="H74" s="36" t="s">
         <v>299</v>
@@ -6535,7 +6554,7 @@
       <c r="E75" s="35" t="s">
         <v>123</v>
       </c>
-      <c r="F75" s="79"/>
+      <c r="F75" s="62"/>
       <c r="G75" s="29"/>
       <c r="H75" s="36" t="s">
         <v>299</v>
@@ -6562,7 +6581,7 @@
       <c r="E76" s="35" t="s">
         <v>123</v>
       </c>
-      <c r="F76" s="79"/>
+      <c r="F76" s="62"/>
       <c r="G76" s="29"/>
       <c r="H76" s="36" t="s">
         <v>299</v>
@@ -6589,7 +6608,7 @@
       <c r="E77" s="35" t="s">
         <v>123</v>
       </c>
-      <c r="F77" s="79"/>
+      <c r="F77" s="62"/>
       <c r="G77" s="29"/>
       <c r="H77" s="36" t="s">
         <v>299</v>
@@ -6616,7 +6635,7 @@
       <c r="E78" s="35" t="s">
         <v>123</v>
       </c>
-      <c r="F78" s="79"/>
+      <c r="F78" s="62"/>
       <c r="G78" s="29"/>
       <c r="H78" s="36" t="s">
         <v>299</v>
@@ -6643,7 +6662,7 @@
       <c r="E79" s="35" t="s">
         <v>123</v>
       </c>
-      <c r="F79" s="79"/>
+      <c r="F79" s="62"/>
       <c r="G79" s="29"/>
       <c r="H79" s="36" t="s">
         <v>299</v>
@@ -6670,7 +6689,7 @@
       <c r="E80" s="35" t="s">
         <v>123</v>
       </c>
-      <c r="F80" s="79"/>
+      <c r="F80" s="62"/>
       <c r="G80" s="29"/>
       <c r="H80" s="36" t="s">
         <v>299</v>
@@ -6697,7 +6716,7 @@
       <c r="E81" s="35" t="s">
         <v>123</v>
       </c>
-      <c r="F81" s="79"/>
+      <c r="F81" s="62"/>
       <c r="G81" s="29"/>
       <c r="H81" s="36" t="s">
         <v>299</v>
@@ -6724,7 +6743,7 @@
       <c r="E82" s="35" t="s">
         <v>282</v>
       </c>
-      <c r="F82" s="79"/>
+      <c r="F82" s="62"/>
       <c r="G82" s="29"/>
       <c r="H82" s="36" t="s">
         <v>299</v>
@@ -6751,7 +6770,7 @@
       <c r="E83" s="35" t="s">
         <v>282</v>
       </c>
-      <c r="F83" s="79"/>
+      <c r="F83" s="62"/>
       <c r="G83" s="29"/>
       <c r="H83" s="36" t="s">
         <v>299</v>
@@ -6778,7 +6797,7 @@
       <c r="E84" s="35" t="s">
         <v>282</v>
       </c>
-      <c r="F84" s="79"/>
+      <c r="F84" s="62"/>
       <c r="G84" s="29"/>
       <c r="H84" s="36" t="s">
         <v>299</v>
@@ -8170,27 +8189,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="62" t="s">
+      <c r="A1" s="63" t="s">
         <v>293</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="64"/>
+      <c r="B1" s="64"/>
+      <c r="C1" s="64"/>
+      <c r="D1" s="64"/>
+      <c r="E1" s="65"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="65"/>
-      <c r="B2" s="66"/>
-      <c r="C2" s="66"/>
-      <c r="D2" s="66"/>
-      <c r="E2" s="67"/>
+      <c r="A2" s="66"/>
+      <c r="B2" s="67"/>
+      <c r="C2" s="67"/>
+      <c r="D2" s="67"/>
+      <c r="E2" s="68"/>
     </row>
     <row r="3" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="68"/>
-      <c r="B3" s="69"/>
-      <c r="C3" s="69"/>
-      <c r="D3" s="69"/>
-      <c r="E3" s="70"/>
+      <c r="A3" s="69"/>
+      <c r="B3" s="70"/>
+      <c r="C3" s="70"/>
+      <c r="D3" s="70"/>
+      <c r="E3" s="71"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -8360,72 +8379,72 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="62" t="s">
+      <c r="A1" s="63" t="s">
         <v>289</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="64"/>
+      <c r="B1" s="64"/>
+      <c r="C1" s="64"/>
+      <c r="D1" s="64"/>
+      <c r="E1" s="65"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="65"/>
-      <c r="B2" s="66"/>
-      <c r="C2" s="66"/>
-      <c r="D2" s="66"/>
-      <c r="E2" s="67"/>
+      <c r="A2" s="66"/>
+      <c r="B2" s="67"/>
+      <c r="C2" s="67"/>
+      <c r="D2" s="67"/>
+      <c r="E2" s="68"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="65"/>
-      <c r="B3" s="66"/>
-      <c r="C3" s="66"/>
-      <c r="D3" s="66"/>
-      <c r="E3" s="67"/>
+      <c r="A3" s="66"/>
+      <c r="B3" s="67"/>
+      <c r="C3" s="67"/>
+      <c r="D3" s="67"/>
+      <c r="E3" s="68"/>
     </row>
     <row r="4" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="68"/>
-      <c r="B4" s="69"/>
-      <c r="C4" s="69"/>
-      <c r="D4" s="69"/>
-      <c r="E4" s="70"/>
+      <c r="A4" s="69"/>
+      <c r="B4" s="70"/>
+      <c r="C4" s="70"/>
+      <c r="D4" s="70"/>
+      <c r="E4" s="71"/>
     </row>
     <row r="5" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="62" t="s">
+      <c r="A6" s="63" t="s">
         <v>290</v>
       </c>
-      <c r="B6" s="71"/>
-      <c r="C6" s="71"/>
-      <c r="D6" s="71"/>
-      <c r="E6" s="72"/>
+      <c r="B6" s="72"/>
+      <c r="C6" s="72"/>
+      <c r="D6" s="72"/>
+      <c r="E6" s="73"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="73"/>
-      <c r="B7" s="74"/>
-      <c r="C7" s="74"/>
-      <c r="D7" s="74"/>
-      <c r="E7" s="75"/>
+      <c r="A7" s="74"/>
+      <c r="B7" s="75"/>
+      <c r="C7" s="75"/>
+      <c r="D7" s="75"/>
+      <c r="E7" s="76"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="73"/>
-      <c r="B8" s="74"/>
-      <c r="C8" s="74"/>
-      <c r="D8" s="74"/>
-      <c r="E8" s="75"/>
+      <c r="A8" s="74"/>
+      <c r="B8" s="75"/>
+      <c r="C8" s="75"/>
+      <c r="D8" s="75"/>
+      <c r="E8" s="76"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="73"/>
-      <c r="B9" s="74"/>
-      <c r="C9" s="74"/>
-      <c r="D9" s="74"/>
-      <c r="E9" s="75"/>
+      <c r="A9" s="74"/>
+      <c r="B9" s="75"/>
+      <c r="C9" s="75"/>
+      <c r="D9" s="75"/>
+      <c r="E9" s="76"/>
     </row>
     <row r="10" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="76"/>
-      <c r="B10" s="77"/>
-      <c r="C10" s="77"/>
-      <c r="D10" s="77"/>
-      <c r="E10" s="78"/>
+      <c r="A10" s="77"/>
+      <c r="B10" s="78"/>
+      <c r="C10" s="78"/>
+      <c r="D10" s="78"/>
+      <c r="E10" s="79"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
@@ -9254,46 +9273,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="62" t="s">
+      <c r="A1" s="63" t="s">
         <v>287</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="64"/>
+      <c r="B1" s="64"/>
+      <c r="C1" s="64"/>
+      <c r="D1" s="64"/>
+      <c r="E1" s="64"/>
+      <c r="F1" s="65"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="65"/>
-      <c r="B2" s="66"/>
-      <c r="C2" s="66"/>
-      <c r="D2" s="66"/>
-      <c r="E2" s="66"/>
-      <c r="F2" s="67"/>
+      <c r="A2" s="66"/>
+      <c r="B2" s="67"/>
+      <c r="C2" s="67"/>
+      <c r="D2" s="67"/>
+      <c r="E2" s="67"/>
+      <c r="F2" s="68"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="65"/>
-      <c r="B3" s="66"/>
-      <c r="C3" s="66"/>
-      <c r="D3" s="66"/>
-      <c r="E3" s="66"/>
-      <c r="F3" s="67"/>
+      <c r="A3" s="66"/>
+      <c r="B3" s="67"/>
+      <c r="C3" s="67"/>
+      <c r="D3" s="67"/>
+      <c r="E3" s="67"/>
+      <c r="F3" s="68"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="65"/>
-      <c r="B4" s="66"/>
-      <c r="C4" s="66"/>
-      <c r="D4" s="66"/>
-      <c r="E4" s="66"/>
-      <c r="F4" s="67"/>
+      <c r="A4" s="66"/>
+      <c r="B4" s="67"/>
+      <c r="C4" s="67"/>
+      <c r="D4" s="67"/>
+      <c r="E4" s="67"/>
+      <c r="F4" s="68"/>
     </row>
     <row r="5" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="68"/>
-      <c r="B5" s="69"/>
-      <c r="C5" s="69"/>
-      <c r="D5" s="69"/>
-      <c r="E5" s="69"/>
-      <c r="F5" s="70"/>
+      <c r="A5" s="69"/>
+      <c r="B5" s="70"/>
+      <c r="C5" s="70"/>
+      <c r="D5" s="70"/>
+      <c r="E5" s="70"/>
+      <c r="F5" s="71"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="18"/>
@@ -9420,83 +9439,83 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8FAEA09-6CEA-024D-AB54-2470DDA2FDE1}">
-  <dimension ref="A1:I17"/>
+  <dimension ref="A1:L17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N14" sqref="N14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="62" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A1" s="63" t="s">
         <v>285</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
-      <c r="G1" s="63"/>
-      <c r="H1" s="63"/>
-      <c r="I1" s="64"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="65"/>
-      <c r="B2" s="66"/>
-      <c r="C2" s="66"/>
-      <c r="D2" s="66"/>
-      <c r="E2" s="66"/>
-      <c r="F2" s="66"/>
-      <c r="G2" s="66"/>
-      <c r="H2" s="66"/>
-      <c r="I2" s="67"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="65"/>
-      <c r="B3" s="66"/>
-      <c r="C3" s="66"/>
-      <c r="D3" s="66"/>
-      <c r="E3" s="66"/>
-      <c r="F3" s="66"/>
-      <c r="G3" s="66"/>
-      <c r="H3" s="66"/>
-      <c r="I3" s="67"/>
-    </row>
-    <row r="4" spans="1:9" ht="13" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="65"/>
-      <c r="B4" s="66"/>
-      <c r="C4" s="66"/>
-      <c r="D4" s="66"/>
-      <c r="E4" s="66"/>
-      <c r="F4" s="66"/>
-      <c r="G4" s="66"/>
-      <c r="H4" s="66"/>
-      <c r="I4" s="67"/>
-    </row>
-    <row r="5" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="65"/>
-      <c r="B5" s="66"/>
-      <c r="C5" s="66"/>
-      <c r="D5" s="66"/>
-      <c r="E5" s="66"/>
-      <c r="F5" s="66"/>
-      <c r="G5" s="66"/>
-      <c r="H5" s="66"/>
-      <c r="I5" s="67"/>
-    </row>
-    <row r="6" spans="1:9" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="68"/>
-      <c r="B6" s="69"/>
-      <c r="C6" s="69"/>
-      <c r="D6" s="69"/>
-      <c r="E6" s="69"/>
-      <c r="F6" s="69"/>
-      <c r="G6" s="69"/>
-      <c r="H6" s="69"/>
-      <c r="I6" s="70"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B1" s="64"/>
+      <c r="C1" s="64"/>
+      <c r="D1" s="64"/>
+      <c r="E1" s="64"/>
+      <c r="F1" s="64"/>
+      <c r="G1" s="64"/>
+      <c r="H1" s="64"/>
+      <c r="I1" s="65"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2" s="66"/>
+      <c r="B2" s="67"/>
+      <c r="C2" s="67"/>
+      <c r="D2" s="67"/>
+      <c r="E2" s="67"/>
+      <c r="F2" s="67"/>
+      <c r="G2" s="67"/>
+      <c r="H2" s="67"/>
+      <c r="I2" s="68"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A3" s="66"/>
+      <c r="B3" s="67"/>
+      <c r="C3" s="67"/>
+      <c r="D3" s="67"/>
+      <c r="E3" s="67"/>
+      <c r="F3" s="67"/>
+      <c r="G3" s="67"/>
+      <c r="H3" s="67"/>
+      <c r="I3" s="68"/>
+    </row>
+    <row r="4" spans="1:12" ht="13" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="66"/>
+      <c r="B4" s="67"/>
+      <c r="C4" s="67"/>
+      <c r="D4" s="67"/>
+      <c r="E4" s="67"/>
+      <c r="F4" s="67"/>
+      <c r="G4" s="67"/>
+      <c r="H4" s="67"/>
+      <c r="I4" s="68"/>
+    </row>
+    <row r="5" spans="1:12" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="66"/>
+      <c r="B5" s="67"/>
+      <c r="C5" s="67"/>
+      <c r="D5" s="67"/>
+      <c r="E5" s="67"/>
+      <c r="F5" s="67"/>
+      <c r="G5" s="67"/>
+      <c r="H5" s="67"/>
+      <c r="I5" s="68"/>
+    </row>
+    <row r="6" spans="1:12" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="69"/>
+      <c r="B6" s="70"/>
+      <c r="C6" s="70"/>
+      <c r="D6" s="70"/>
+      <c r="E6" s="70"/>
+      <c r="F6" s="70"/>
+      <c r="G6" s="70"/>
+      <c r="H6" s="70"/>
+      <c r="I6" s="71"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>90</v>
       </c>
@@ -9518,8 +9537,14 @@
       <c r="I9" t="s">
         <v>463</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K9" s="1" t="s">
+        <v>480</v>
+      </c>
+      <c r="L9" s="16" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="20" t="s">
         <v>23</v>
       </c>
@@ -9538,8 +9563,14 @@
       <c r="H10" s="20" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K10" s="21" t="s">
+        <v>476</v>
+      </c>
+      <c r="L10" s="22" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="20" t="s">
         <v>295</v>
       </c>
@@ -9558,8 +9589,14 @@
       <c r="H11" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K11" s="23" t="s">
+        <v>477</v>
+      </c>
+      <c r="L11" s="24" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>91</v>
       </c>
@@ -9575,8 +9612,14 @@
       <c r="H12" s="20" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K12" s="82" t="s">
+        <v>478</v>
+      </c>
+      <c r="L12" s="83" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>92</v>
       </c>
@@ -9592,8 +9635,14 @@
       <c r="H13" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K13" s="80" t="s">
+        <v>37</v>
+      </c>
+      <c r="L13" s="81" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>93</v>
       </c>
@@ -9609,8 +9658,14 @@
       <c r="H14" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K14" s="82" t="s">
+        <v>36</v>
+      </c>
+      <c r="L14" s="83" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>94</v>
       </c>
@@ -9623,22 +9678,32 @@
       <c r="H15" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K15" s="80" t="s">
+        <v>479</v>
+      </c>
+      <c r="L15" s="81" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>95</v>
       </c>
       <c r="B16" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="K16" s="82"/>
+      <c r="L16" s="83"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>96</v>
       </c>
       <c r="B17" t="s">
         <v>43</v>
       </c>
+      <c r="K17" s="80"/>
+      <c r="L17" s="81"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -9673,47 +9738,47 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="62" t="s">
+      <c r="A1" s="63" t="s">
         <v>288</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="64"/>
+      <c r="B1" s="64"/>
+      <c r="C1" s="64"/>
+      <c r="D1" s="64"/>
+      <c r="E1" s="64"/>
+      <c r="F1" s="65"/>
     </row>
     <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="65"/>
-      <c r="B2" s="66"/>
-      <c r="C2" s="66"/>
-      <c r="D2" s="66"/>
-      <c r="E2" s="66"/>
-      <c r="F2" s="67"/>
+      <c r="A2" s="66"/>
+      <c r="B2" s="67"/>
+      <c r="C2" s="67"/>
+      <c r="D2" s="67"/>
+      <c r="E2" s="67"/>
+      <c r="F2" s="68"/>
     </row>
     <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="65"/>
-      <c r="B3" s="66"/>
-      <c r="C3" s="66"/>
-      <c r="D3" s="66"/>
-      <c r="E3" s="66"/>
-      <c r="F3" s="67"/>
+      <c r="A3" s="66"/>
+      <c r="B3" s="67"/>
+      <c r="C3" s="67"/>
+      <c r="D3" s="67"/>
+      <c r="E3" s="67"/>
+      <c r="F3" s="68"/>
     </row>
     <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="65"/>
-      <c r="B4" s="66"/>
-      <c r="C4" s="66"/>
-      <c r="D4" s="66"/>
-      <c r="E4" s="66"/>
-      <c r="F4" s="67"/>
+      <c r="A4" s="66"/>
+      <c r="B4" s="67"/>
+      <c r="C4" s="67"/>
+      <c r="D4" s="67"/>
+      <c r="E4" s="67"/>
+      <c r="F4" s="68"/>
       <c r="G4" s="17"/>
     </row>
     <row r="5" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="68"/>
-      <c r="B5" s="69"/>
-      <c r="C5" s="69"/>
-      <c r="D5" s="69"/>
-      <c r="E5" s="69"/>
-      <c r="F5" s="70"/>
+      <c r="A5" s="69"/>
+      <c r="B5" s="70"/>
+      <c r="C5" s="70"/>
+      <c r="D5" s="70"/>
+      <c r="E5" s="70"/>
+      <c r="F5" s="71"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
@@ -9883,105 +9948,105 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="62" t="s">
+      <c r="A1" s="63" t="s">
         <v>292</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
-      <c r="G1" s="63"/>
-      <c r="H1" s="63"/>
-      <c r="I1" s="64"/>
+      <c r="B1" s="64"/>
+      <c r="C1" s="64"/>
+      <c r="D1" s="64"/>
+      <c r="E1" s="64"/>
+      <c r="F1" s="64"/>
+      <c r="G1" s="64"/>
+      <c r="H1" s="64"/>
+      <c r="I1" s="65"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="65"/>
-      <c r="B2" s="66"/>
-      <c r="C2" s="66"/>
-      <c r="D2" s="66"/>
-      <c r="E2" s="66"/>
-      <c r="F2" s="66"/>
-      <c r="G2" s="66"/>
-      <c r="H2" s="66"/>
-      <c r="I2" s="67"/>
+      <c r="A2" s="66"/>
+      <c r="B2" s="67"/>
+      <c r="C2" s="67"/>
+      <c r="D2" s="67"/>
+      <c r="E2" s="67"/>
+      <c r="F2" s="67"/>
+      <c r="G2" s="67"/>
+      <c r="H2" s="67"/>
+      <c r="I2" s="68"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="65"/>
-      <c r="B3" s="66"/>
-      <c r="C3" s="66"/>
-      <c r="D3" s="66"/>
-      <c r="E3" s="66"/>
-      <c r="F3" s="66"/>
-      <c r="G3" s="66"/>
-      <c r="H3" s="66"/>
-      <c r="I3" s="67"/>
+      <c r="A3" s="66"/>
+      <c r="B3" s="67"/>
+      <c r="C3" s="67"/>
+      <c r="D3" s="67"/>
+      <c r="E3" s="67"/>
+      <c r="F3" s="67"/>
+      <c r="G3" s="67"/>
+      <c r="H3" s="67"/>
+      <c r="I3" s="68"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="65"/>
-      <c r="B4" s="66"/>
-      <c r="C4" s="66"/>
-      <c r="D4" s="66"/>
-      <c r="E4" s="66"/>
-      <c r="F4" s="66"/>
-      <c r="G4" s="66"/>
-      <c r="H4" s="66"/>
-      <c r="I4" s="67"/>
+      <c r="A4" s="66"/>
+      <c r="B4" s="67"/>
+      <c r="C4" s="67"/>
+      <c r="D4" s="67"/>
+      <c r="E4" s="67"/>
+      <c r="F4" s="67"/>
+      <c r="G4" s="67"/>
+      <c r="H4" s="67"/>
+      <c r="I4" s="68"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="65"/>
-      <c r="B5" s="66"/>
-      <c r="C5" s="66"/>
-      <c r="D5" s="66"/>
-      <c r="E5" s="66"/>
-      <c r="F5" s="66"/>
-      <c r="G5" s="66"/>
-      <c r="H5" s="66"/>
-      <c r="I5" s="67"/>
+      <c r="A5" s="66"/>
+      <c r="B5" s="67"/>
+      <c r="C5" s="67"/>
+      <c r="D5" s="67"/>
+      <c r="E5" s="67"/>
+      <c r="F5" s="67"/>
+      <c r="G5" s="67"/>
+      <c r="H5" s="67"/>
+      <c r="I5" s="68"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="65"/>
-      <c r="B6" s="66"/>
-      <c r="C6" s="66"/>
-      <c r="D6" s="66"/>
-      <c r="E6" s="66"/>
-      <c r="F6" s="66"/>
-      <c r="G6" s="66"/>
-      <c r="H6" s="66"/>
-      <c r="I6" s="67"/>
+      <c r="A6" s="66"/>
+      <c r="B6" s="67"/>
+      <c r="C6" s="67"/>
+      <c r="D6" s="67"/>
+      <c r="E6" s="67"/>
+      <c r="F6" s="67"/>
+      <c r="G6" s="67"/>
+      <c r="H6" s="67"/>
+      <c r="I6" s="68"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="65"/>
-      <c r="B7" s="66"/>
-      <c r="C7" s="66"/>
-      <c r="D7" s="66"/>
-      <c r="E7" s="66"/>
-      <c r="F7" s="66"/>
-      <c r="G7" s="66"/>
-      <c r="H7" s="66"/>
-      <c r="I7" s="67"/>
+      <c r="A7" s="66"/>
+      <c r="B7" s="67"/>
+      <c r="C7" s="67"/>
+      <c r="D7" s="67"/>
+      <c r="E7" s="67"/>
+      <c r="F7" s="67"/>
+      <c r="G7" s="67"/>
+      <c r="H7" s="67"/>
+      <c r="I7" s="68"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="65"/>
-      <c r="B8" s="66"/>
-      <c r="C8" s="66"/>
-      <c r="D8" s="66"/>
-      <c r="E8" s="66"/>
-      <c r="F8" s="66"/>
-      <c r="G8" s="66"/>
-      <c r="H8" s="66"/>
-      <c r="I8" s="67"/>
+      <c r="A8" s="66"/>
+      <c r="B8" s="67"/>
+      <c r="C8" s="67"/>
+      <c r="D8" s="67"/>
+      <c r="E8" s="67"/>
+      <c r="F8" s="67"/>
+      <c r="G8" s="67"/>
+      <c r="H8" s="67"/>
+      <c r="I8" s="68"/>
     </row>
     <row r="9" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="68"/>
-      <c r="B9" s="69"/>
-      <c r="C9" s="69"/>
-      <c r="D9" s="69"/>
-      <c r="E9" s="69"/>
-      <c r="F9" s="69"/>
-      <c r="G9" s="69"/>
-      <c r="H9" s="69"/>
-      <c r="I9" s="70"/>
+      <c r="A9" s="69"/>
+      <c r="B9" s="70"/>
+      <c r="C9" s="70"/>
+      <c r="D9" s="70"/>
+      <c r="E9" s="70"/>
+      <c r="F9" s="70"/>
+      <c r="G9" s="70"/>
+      <c r="H9" s="70"/>
+      <c r="I9" s="71"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -10012,41 +10077,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="62" t="s">
+      <c r="A1" s="63" t="s">
         <v>286</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="64"/>
+      <c r="B1" s="64"/>
+      <c r="C1" s="64"/>
+      <c r="D1" s="64"/>
+      <c r="E1" s="65"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="65"/>
-      <c r="B2" s="66"/>
-      <c r="C2" s="66"/>
-      <c r="D2" s="66"/>
-      <c r="E2" s="67"/>
+      <c r="A2" s="66"/>
+      <c r="B2" s="67"/>
+      <c r="C2" s="67"/>
+      <c r="D2" s="67"/>
+      <c r="E2" s="68"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="65"/>
-      <c r="B3" s="66"/>
-      <c r="C3" s="66"/>
-      <c r="D3" s="66"/>
-      <c r="E3" s="67"/>
+      <c r="A3" s="66"/>
+      <c r="B3" s="67"/>
+      <c r="C3" s="67"/>
+      <c r="D3" s="67"/>
+      <c r="E3" s="68"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="65"/>
-      <c r="B4" s="66"/>
-      <c r="C4" s="66"/>
-      <c r="D4" s="66"/>
-      <c r="E4" s="67"/>
+      <c r="A4" s="66"/>
+      <c r="B4" s="67"/>
+      <c r="C4" s="67"/>
+      <c r="D4" s="67"/>
+      <c r="E4" s="68"/>
     </row>
     <row r="5" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="68"/>
-      <c r="B5" s="69"/>
-      <c r="C5" s="69"/>
-      <c r="D5" s="69"/>
-      <c r="E5" s="70"/>
+      <c r="A5" s="69"/>
+      <c r="B5" s="70"/>
+      <c r="C5" s="70"/>
+      <c r="D5" s="70"/>
+      <c r="E5" s="71"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
@@ -10402,159 +10467,159 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="62" t="s">
+      <c r="A1" s="63" t="s">
         <v>291</v>
       </c>
-      <c r="B1" s="71"/>
-      <c r="C1" s="71"/>
-      <c r="D1" s="71"/>
-      <c r="E1" s="71"/>
-      <c r="F1" s="71"/>
-      <c r="G1" s="71"/>
-      <c r="H1" s="71"/>
-      <c r="I1" s="71"/>
-      <c r="J1" s="71"/>
-      <c r="K1" s="72"/>
+      <c r="B1" s="72"/>
+      <c r="C1" s="72"/>
+      <c r="D1" s="72"/>
+      <c r="E1" s="72"/>
+      <c r="F1" s="72"/>
+      <c r="G1" s="72"/>
+      <c r="H1" s="72"/>
+      <c r="I1" s="72"/>
+      <c r="J1" s="72"/>
+      <c r="K1" s="73"/>
       <c r="L1" s="19"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A2" s="73"/>
-      <c r="B2" s="74"/>
-      <c r="C2" s="74"/>
-      <c r="D2" s="74"/>
-      <c r="E2" s="74"/>
-      <c r="F2" s="74"/>
-      <c r="G2" s="74"/>
-      <c r="H2" s="74"/>
-      <c r="I2" s="74"/>
-      <c r="J2" s="74"/>
-      <c r="K2" s="75"/>
+      <c r="A2" s="74"/>
+      <c r="B2" s="75"/>
+      <c r="C2" s="75"/>
+      <c r="D2" s="75"/>
+      <c r="E2" s="75"/>
+      <c r="F2" s="75"/>
+      <c r="G2" s="75"/>
+      <c r="H2" s="75"/>
+      <c r="I2" s="75"/>
+      <c r="J2" s="75"/>
+      <c r="K2" s="76"/>
       <c r="L2" s="19"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A3" s="73"/>
-      <c r="B3" s="74"/>
-      <c r="C3" s="74"/>
-      <c r="D3" s="74"/>
-      <c r="E3" s="74"/>
-      <c r="F3" s="74"/>
-      <c r="G3" s="74"/>
-      <c r="H3" s="74"/>
-      <c r="I3" s="74"/>
-      <c r="J3" s="74"/>
-      <c r="K3" s="75"/>
+      <c r="A3" s="74"/>
+      <c r="B3" s="75"/>
+      <c r="C3" s="75"/>
+      <c r="D3" s="75"/>
+      <c r="E3" s="75"/>
+      <c r="F3" s="75"/>
+      <c r="G3" s="75"/>
+      <c r="H3" s="75"/>
+      <c r="I3" s="75"/>
+      <c r="J3" s="75"/>
+      <c r="K3" s="76"/>
       <c r="L3" s="19"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A4" s="73"/>
-      <c r="B4" s="74"/>
-      <c r="C4" s="74"/>
-      <c r="D4" s="74"/>
-      <c r="E4" s="74"/>
-      <c r="F4" s="74"/>
-      <c r="G4" s="74"/>
-      <c r="H4" s="74"/>
-      <c r="I4" s="74"/>
-      <c r="J4" s="74"/>
-      <c r="K4" s="75"/>
+      <c r="A4" s="74"/>
+      <c r="B4" s="75"/>
+      <c r="C4" s="75"/>
+      <c r="D4" s="75"/>
+      <c r="E4" s="75"/>
+      <c r="F4" s="75"/>
+      <c r="G4" s="75"/>
+      <c r="H4" s="75"/>
+      <c r="I4" s="75"/>
+      <c r="J4" s="75"/>
+      <c r="K4" s="76"/>
       <c r="L4" s="19"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A5" s="73"/>
-      <c r="B5" s="74"/>
-      <c r="C5" s="74"/>
-      <c r="D5" s="74"/>
-      <c r="E5" s="74"/>
-      <c r="F5" s="74"/>
-      <c r="G5" s="74"/>
-      <c r="H5" s="74"/>
-      <c r="I5" s="74"/>
-      <c r="J5" s="74"/>
-      <c r="K5" s="75"/>
+      <c r="A5" s="74"/>
+      <c r="B5" s="75"/>
+      <c r="C5" s="75"/>
+      <c r="D5" s="75"/>
+      <c r="E5" s="75"/>
+      <c r="F5" s="75"/>
+      <c r="G5" s="75"/>
+      <c r="H5" s="75"/>
+      <c r="I5" s="75"/>
+      <c r="J5" s="75"/>
+      <c r="K5" s="76"/>
       <c r="L5" s="19"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A6" s="73"/>
-      <c r="B6" s="74"/>
-      <c r="C6" s="74"/>
-      <c r="D6" s="74"/>
-      <c r="E6" s="74"/>
-      <c r="F6" s="74"/>
-      <c r="G6" s="74"/>
-      <c r="H6" s="74"/>
-      <c r="I6" s="74"/>
-      <c r="J6" s="74"/>
-      <c r="K6" s="75"/>
+      <c r="A6" s="74"/>
+      <c r="B6" s="75"/>
+      <c r="C6" s="75"/>
+      <c r="D6" s="75"/>
+      <c r="E6" s="75"/>
+      <c r="F6" s="75"/>
+      <c r="G6" s="75"/>
+      <c r="H6" s="75"/>
+      <c r="I6" s="75"/>
+      <c r="J6" s="75"/>
+      <c r="K6" s="76"/>
       <c r="L6" s="19"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A7" s="73"/>
-      <c r="B7" s="74"/>
-      <c r="C7" s="74"/>
-      <c r="D7" s="74"/>
-      <c r="E7" s="74"/>
-      <c r="F7" s="74"/>
-      <c r="G7" s="74"/>
-      <c r="H7" s="74"/>
-      <c r="I7" s="74"/>
-      <c r="J7" s="74"/>
-      <c r="K7" s="75"/>
+      <c r="A7" s="74"/>
+      <c r="B7" s="75"/>
+      <c r="C7" s="75"/>
+      <c r="D7" s="75"/>
+      <c r="E7" s="75"/>
+      <c r="F7" s="75"/>
+      <c r="G7" s="75"/>
+      <c r="H7" s="75"/>
+      <c r="I7" s="75"/>
+      <c r="J7" s="75"/>
+      <c r="K7" s="76"/>
       <c r="L7" s="19"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A8" s="73"/>
-      <c r="B8" s="74"/>
-      <c r="C8" s="74"/>
-      <c r="D8" s="74"/>
-      <c r="E8" s="74"/>
-      <c r="F8" s="74"/>
-      <c r="G8" s="74"/>
-      <c r="H8" s="74"/>
-      <c r="I8" s="74"/>
-      <c r="J8" s="74"/>
-      <c r="K8" s="75"/>
+      <c r="A8" s="74"/>
+      <c r="B8" s="75"/>
+      <c r="C8" s="75"/>
+      <c r="D8" s="75"/>
+      <c r="E8" s="75"/>
+      <c r="F8" s="75"/>
+      <c r="G8" s="75"/>
+      <c r="H8" s="75"/>
+      <c r="I8" s="75"/>
+      <c r="J8" s="75"/>
+      <c r="K8" s="76"/>
       <c r="L8" s="19"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A9" s="73"/>
-      <c r="B9" s="74"/>
-      <c r="C9" s="74"/>
-      <c r="D9" s="74"/>
-      <c r="E9" s="74"/>
-      <c r="F9" s="74"/>
-      <c r="G9" s="74"/>
-      <c r="H9" s="74"/>
-      <c r="I9" s="74"/>
-      <c r="J9" s="74"/>
-      <c r="K9" s="75"/>
+      <c r="A9" s="74"/>
+      <c r="B9" s="75"/>
+      <c r="C9" s="75"/>
+      <c r="D9" s="75"/>
+      <c r="E9" s="75"/>
+      <c r="F9" s="75"/>
+      <c r="G9" s="75"/>
+      <c r="H9" s="75"/>
+      <c r="I9" s="75"/>
+      <c r="J9" s="75"/>
+      <c r="K9" s="76"/>
       <c r="L9" s="19"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A10" s="73"/>
-      <c r="B10" s="74"/>
-      <c r="C10" s="74"/>
-      <c r="D10" s="74"/>
-      <c r="E10" s="74"/>
-      <c r="F10" s="74"/>
-      <c r="G10" s="74"/>
-      <c r="H10" s="74"/>
-      <c r="I10" s="74"/>
-      <c r="J10" s="74"/>
-      <c r="K10" s="75"/>
+      <c r="A10" s="74"/>
+      <c r="B10" s="75"/>
+      <c r="C10" s="75"/>
+      <c r="D10" s="75"/>
+      <c r="E10" s="75"/>
+      <c r="F10" s="75"/>
+      <c r="G10" s="75"/>
+      <c r="H10" s="75"/>
+      <c r="I10" s="75"/>
+      <c r="J10" s="75"/>
+      <c r="K10" s="76"/>
       <c r="L10" s="19"/>
     </row>
     <row r="11" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="76"/>
-      <c r="B11" s="77"/>
-      <c r="C11" s="77"/>
-      <c r="D11" s="77"/>
-      <c r="E11" s="77"/>
-      <c r="F11" s="77"/>
-      <c r="G11" s="77"/>
-      <c r="H11" s="77"/>
-      <c r="I11" s="77"/>
-      <c r="J11" s="77"/>
-      <c r="K11" s="78"/>
+      <c r="A11" s="77"/>
+      <c r="B11" s="78"/>
+      <c r="C11" s="78"/>
+      <c r="D11" s="78"/>
+      <c r="E11" s="78"/>
+      <c r="F11" s="78"/>
+      <c r="G11" s="78"/>
+      <c r="H11" s="78"/>
+      <c r="I11" s="78"/>
+      <c r="J11" s="78"/>
+      <c r="K11" s="79"/>
       <c r="L11" s="19"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">

</xml_diff>